<commit_message>
added new budget, config, pic 9
</commit_message>
<xml_diff>
--- a/input/budget.xlsx
+++ b/input/budget.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4784027176d9b30c/_KMONITOR/_KÖKÖ/TERÉZVÁROS_KÖKÖ/2021_budget_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1015" documentId="8_{E24534E0-E60B-4E45-949D-D5E79B4883FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0409EED2-3BBA-492A-A2B4-152942588857}"/>
+  <xr:revisionPtr revIDLastSave="1020" documentId="8_{E24534E0-E60B-4E45-949D-D5E79B4883FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{97C4DC14-F2C5-4E89-B6D7-4254112EA5D8}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{501F2212-62D4-412E-9A6C-EB2F87D26B78}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="518" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="384">
   <si>
     <t>Megnevezés</t>
   </si>
@@ -98,9 +98,6 @@
     <t>Egyéb közhatalmi bevételek (díjak, bírságok, pótlékok ) (B25)</t>
   </si>
   <si>
-    <t>Működési bevételek (B3)</t>
-  </si>
-  <si>
     <t>Nyújtott szolgáltatás ellenértéke (B31)</t>
   </si>
   <si>
@@ -143,27 +140,6 @@
     <t>Kamatbevételek (B37)</t>
   </si>
   <si>
-    <t>Működési célú átvett átvett pénzeszközök (B4)</t>
-  </si>
-  <si>
-    <t>Felhalmozási célú támogatás államháztartáson belülről (B5)</t>
-  </si>
-  <si>
-    <t>Felhalmozási  bevételek (B6)</t>
-  </si>
-  <si>
-    <t>Ingatlanok értékesítése (B61)</t>
-  </si>
-  <si>
-    <t>Felhalmozási célú átvett pénzeszközök (B7)</t>
-  </si>
-  <si>
-    <t>Finanszírozási bevételek (B8)</t>
-  </si>
-  <si>
-    <t>Maradvány igénybevétele (B81)</t>
-  </si>
-  <si>
     <t>Finanszírozási többlet (maradvány) (FT1)</t>
   </si>
   <si>
@@ -329,9 +305,6 @@
     <t>Szolgáltatási kiadások (K2103)</t>
   </si>
   <si>
-    <t>Kiküldetés, reklám (K2104)</t>
-  </si>
-  <si>
     <t>Különféle befizetések és dologi kiadások (K2105)</t>
   </si>
   <si>
@@ -707,9 +680,6 @@
     <t>Szolgáltatási kiadások (K2203)</t>
   </si>
   <si>
-    <t>Kiküldetés, reklám (K2204)</t>
-  </si>
-  <si>
     <t>Különféle befizetések és dologi kiadások (K2205)</t>
   </si>
   <si>
@@ -1197,6 +1167,27 @@
   </si>
   <si>
     <t>Maradvány igénybevétele (B52)</t>
+  </si>
+  <si>
+    <t>Működési célú átvett átvett pénzeszközök (B38)</t>
+  </si>
+  <si>
+    <t>Felhalmozási bevételek, támogatások, átvett pénzeszközök (B4)</t>
+  </si>
+  <si>
+    <t>Felhalmozási célú támogatás államháztartáson belülről (B41)</t>
+  </si>
+  <si>
+    <t>Felhalmozási  bevételek - ingatlanértékesítés (B42)</t>
+  </si>
+  <si>
+    <t>Finanszírozási bevételek - maradvány igénybevétele (B5)</t>
+  </si>
+  <si>
+    <t>Kiküldetés (K2104)</t>
+  </si>
+  <si>
+    <t>Kiküldetés (K2204)</t>
   </si>
 </sst>
 </file>
@@ -1661,8 +1652,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FAB4C5-B3A4-426F-A8BC-E577AEC02B08}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1881,10 +1872,10 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>368</v>
       </c>
       <c r="C18" s="2">
-        <v>3778814700</v>
+        <v>3779214700</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1892,7 +1883,7 @@
         <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C19" s="2">
         <v>71036200</v>
@@ -1903,7 +1894,7 @@
         <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C20" s="2">
         <v>95023800</v>
@@ -1914,7 +1905,7 @@
         <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C21" s="2">
         <v>2269402000</v>
@@ -1925,7 +1916,7 @@
         <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="2">
         <v>400000000</v>
@@ -1937,7 +1928,7 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C23" s="2">
         <v>541100000</v>
@@ -1949,7 +1940,7 @@
         <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C24" s="2">
         <v>130000000</v>
@@ -1961,7 +1952,7 @@
         <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" s="2">
         <v>468000000</v>
@@ -1972,7 +1963,7 @@
         <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" s="2">
         <v>607302000</v>
@@ -1983,7 +1974,7 @@
         <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" s="2">
         <v>64000000</v>
@@ -1994,7 +1985,7 @@
         <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" s="2">
         <v>59000000</v>
@@ -2005,7 +1996,7 @@
         <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" s="2">
         <v>95250000</v>
@@ -2016,7 +2007,7 @@
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="2">
         <v>609741700</v>
@@ -2027,7 +2018,7 @@
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" s="2">
         <v>605361000</v>
@@ -2038,7 +2029,7 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" s="2">
         <v>33000000</v>
@@ -2049,7 +2040,7 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>377</v>
       </c>
       <c r="C33" s="2">
         <v>400000</v>
@@ -2060,10 +2051,10 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>378</v>
       </c>
       <c r="C34" s="2">
-        <v>200000000</v>
+        <v>1060817431</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2071,10 +2062,10 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>379</v>
       </c>
       <c r="C35" s="2">
-        <v>710636000</v>
+        <v>200000000</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2082,7 +2073,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>380</v>
       </c>
       <c r="C36" s="2">
         <v>710636000</v>
@@ -2093,7 +2084,7 @@
         <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>373</v>
       </c>
       <c r="C37" s="2">
         <v>150181431</v>
@@ -2104,7 +2095,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>381</v>
       </c>
       <c r="C38" s="2">
         <v>2826252158</v>
@@ -2115,22 +2106,15 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C39" s="2">
         <v>2826252158</v>
       </c>
     </row>
     <row r="40" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
-        <v>99</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="C40" s="2">
-        <v>2826252158</v>
-      </c>
+      <c r="A40" s="19"/>
+      <c r="C40" s="2"/>
       <c r="D40" s="6"/>
       <c r="E40" s="25"/>
     </row>
@@ -2145,8 +2129,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76BAFE8-6BF8-4E8A-B864-E53778D2F9B3}">
   <dimension ref="A1:F161"/>
   <sheetViews>
-    <sheetView topLeftCell="A144" workbookViewId="0">
-      <selection activeCell="B158" sqref="B158"/>
+    <sheetView topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="D52" sqref="D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2184,7 +2168,7 @@
         <v>99</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C3" s="7">
         <f>C4+C7+C11+C32+C36+C40+C44+C48</f>
@@ -2198,7 +2182,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C4" s="7">
         <f>SUM(C5:C6)</f>
@@ -2211,7 +2195,7 @@
         <v>99</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C5" s="7">
         <v>217908168</v>
@@ -2223,7 +2207,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="7">
         <v>41760014</v>
@@ -2235,7 +2219,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7" s="7">
         <f>SUM(C8:C10)</f>
@@ -2248,7 +2232,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C8" s="7">
         <v>1538081462</v>
@@ -2260,7 +2244,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C9" s="7">
         <v>21615392</v>
@@ -2272,7 +2256,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C10" s="7">
         <v>311812108</v>
@@ -2284,7 +2268,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C11" s="7">
         <f>C12+C16+C20+C24+C28</f>
@@ -2297,7 +2281,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C12" s="7">
         <f>SUM(C13:C15)</f>
@@ -2310,7 +2294,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" s="7">
         <v>77428849</v>
@@ -2322,7 +2306,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C14" s="7">
         <v>900000</v>
@@ -2334,7 +2318,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C15" s="7">
         <v>15287856</v>
@@ -2346,7 +2330,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C16" s="7">
         <f>SUM(C17:C19)</f>
@@ -2359,7 +2343,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" s="7">
         <v>117364155</v>
@@ -2371,7 +2355,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C18" s="7">
         <v>3977000</v>
@@ -2383,7 +2367,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19" s="7">
         <v>25924959</v>
@@ -2395,7 +2379,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C20" s="7">
         <f>SUM(C21:C23)</f>
@@ -2408,7 +2392,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C21" s="7">
         <v>83957303</v>
@@ -2420,7 +2404,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C22" s="7">
         <v>770000</v>
@@ -2432,7 +2416,7 @@
         <v>99</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C23" s="7">
         <v>16541451</v>
@@ -2444,7 +2428,7 @@
         <v>99</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C24" s="7">
         <f>SUM(C25:C27)</f>
@@ -2457,7 +2441,7 @@
         <v>99</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C25" s="7">
         <v>119592948</v>
@@ -2469,7 +2453,7 @@
         <v>99</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C26" s="7">
         <v>1870000</v>
@@ -2481,7 +2465,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C27" s="7">
         <v>26270236</v>
@@ -2493,7 +2477,7 @@
         <v>99</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C28" s="7">
         <f>SUM(C29:C31)</f>
@@ -2506,7 +2490,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C29" s="7">
         <v>113855057</v>
@@ -2518,7 +2502,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C30" s="7">
         <v>2490000</v>
@@ -2530,7 +2514,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C31" s="7">
         <v>24270240</v>
@@ -2542,7 +2526,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C32" s="7">
         <f>SUM(C33:C35)</f>
@@ -2555,7 +2539,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" s="7">
         <v>673123300</v>
@@ -2567,7 +2551,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C34" s="7">
         <v>82875200</v>
@@ -2579,7 +2563,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C35" s="7">
         <v>140844500</v>
@@ -2591,7 +2575,7 @@
         <v>99</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C36" s="7">
         <f>SUM(C37:C39)</f>
@@ -2604,7 +2588,7 @@
         <v>99</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C37" s="7">
         <v>36680461</v>
@@ -2616,7 +2600,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C38" s="7">
         <v>1310000</v>
@@ -2628,7 +2612,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C39" s="7">
         <v>7460588</v>
@@ -2640,7 +2624,7 @@
         <v>99</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C40" s="7">
         <f>SUM(C41:C43)</f>
@@ -2653,7 +2637,7 @@
         <v>99</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C41" s="7">
         <v>237656627</v>
@@ -2665,7 +2649,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C42" s="7">
         <v>5764400</v>
@@ -2677,7 +2661,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C43" s="7">
         <v>53035237</v>
@@ -2689,7 +2673,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C44" s="7">
         <f>SUM(C45:C47)</f>
@@ -2702,7 +2686,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C45" s="7">
         <v>177302965</v>
@@ -2714,7 +2698,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C46" s="7">
         <v>1250000</v>
@@ -2726,7 +2710,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C47" s="7">
         <v>38103017</v>
@@ -2738,7 +2722,7 @@
         <v>99</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C48" s="7">
         <f>SUM(C49:C51)</f>
@@ -2751,7 +2735,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C49" s="7">
         <v>222010984</v>
@@ -2763,7 +2747,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C50" s="7">
         <v>250000</v>
@@ -2775,7 +2759,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C51" s="7">
         <v>47701661</v>
@@ -2787,7 +2771,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C52" s="7">
         <f>C53+C59+C60+C66+C67+C68+C69+C70</f>
@@ -2800,7 +2784,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C53" s="7">
         <v>5287267089</v>
@@ -2812,7 +2796,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C54" s="23">
         <v>29970956</v>
@@ -2824,7 +2808,7 @@
         <v>99</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C55" s="23">
         <v>58065000</v>
@@ -2836,7 +2820,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C56" s="23">
         <v>3451726392</v>
@@ -2848,7 +2832,7 @@
         <v>99</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>97</v>
+        <v>382</v>
       </c>
       <c r="C57" s="23">
         <v>91132500</v>
@@ -2860,7 +2844,7 @@
         <v>99</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C58" s="23">
         <v>1656372241</v>
@@ -2872,7 +2856,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C59" s="7">
         <v>370941077</v>
@@ -2884,7 +2868,7 @@
         <v>99</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C60" s="7">
         <f>SUM(C61:C65)</f>
@@ -2897,7 +2881,7 @@
         <v>99</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C61" s="7">
         <v>10881300</v>
@@ -2909,7 +2893,7 @@
         <v>99</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C62" s="7">
         <v>19492650</v>
@@ -2921,7 +2905,7 @@
         <v>99</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C63" s="7">
         <v>15397500</v>
@@ -2933,7 +2917,7 @@
         <v>99</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C64" s="7">
         <v>15516450</v>
@@ -2945,7 +2929,7 @@
         <v>99</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C65" s="7">
         <v>18880500</v>
@@ -2957,7 +2941,7 @@
         <v>99</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C66" s="7">
         <v>269407000</v>
@@ -2969,7 +2953,7 @@
         <v>99</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C67" s="7">
         <v>13312063</v>
@@ -2981,7 +2965,7 @@
         <v>99</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C68" s="7">
         <v>96503877</v>
@@ -2993,7 +2977,7 @@
         <v>99</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C69" s="7">
         <v>40761893</v>
@@ -3005,7 +2989,7 @@
         <v>99</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C70" s="7">
         <v>61391544</v>
@@ -3017,7 +3001,7 @@
         <v>99</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C71" s="7">
         <f>C72+C73+C74+C75</f>
@@ -3030,7 +3014,7 @@
         <v>99</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C72" s="7">
         <v>374096400</v>
@@ -3042,7 +3026,7 @@
         <v>99</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="C73" s="7">
         <v>120000</v>
@@ -3054,7 +3038,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C74" s="7">
         <v>130000</v>
@@ -3066,7 +3050,7 @@
         <v>99</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="C75" s="7">
         <v>3200000</v>
@@ -3078,7 +3062,7 @@
         <v>99</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C76" s="7">
         <f>C77+C79+C97+C100</f>
@@ -3091,7 +3075,7 @@
         <v>99</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C77" s="7">
         <f>C78</f>
@@ -3104,7 +3088,7 @@
         <v>99</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="C78" s="7">
         <v>38602000</v>
@@ -3116,7 +3100,7 @@
         <v>99</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C79" s="7">
         <f>C80+C81+C82+C83+C93</f>
@@ -3129,7 +3113,7 @@
         <v>99</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="C80" s="7">
         <v>40000000</v>
@@ -3142,7 +3126,7 @@
         <v>99</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="C81" s="7">
         <v>17000000</v>
@@ -3155,7 +3139,7 @@
         <v>99</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C82" s="7">
         <v>6000000</v>
@@ -3168,7 +3152,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="C83" s="7">
         <f>SUM(C84:C92)</f>
@@ -3182,7 +3166,7 @@
         <v>99</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C84" s="7">
         <v>500000</v>
@@ -3195,7 +3179,7 @@
         <v>99</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="C85" s="7">
         <v>500000</v>
@@ -3208,7 +3192,7 @@
         <v>99</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C86" s="7">
         <v>500000</v>
@@ -3221,7 +3205,7 @@
         <v>99</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C87" s="7">
         <v>500000</v>
@@ -3234,7 +3218,7 @@
         <v>99</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C88" s="7">
         <v>500000</v>
@@ -3247,7 +3231,7 @@
         <v>99</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C89" s="7">
         <v>500000</v>
@@ -3260,7 +3244,7 @@
         <v>99</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C90" s="7">
         <v>4000000</v>
@@ -3273,7 +3257,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C91" s="7">
         <v>1000000</v>
@@ -3286,7 +3270,7 @@
         <v>99</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C92" s="7">
         <v>2000000</v>
@@ -3299,7 +3283,7 @@
         <v>99</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C93" s="7">
         <f>SUM(C94:C96)</f>
@@ -3313,7 +3297,7 @@
         <v>99</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C94" s="7">
         <v>217385530</v>
@@ -3326,7 +3310,7 @@
         <v>99</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C95" s="7">
         <v>40000000</v>
@@ -3339,7 +3323,7 @@
         <v>99</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="C96" s="7">
         <v>467138327</v>
@@ -3352,7 +3336,7 @@
         <v>99</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C97" s="7">
         <f>SUM(C98:C99)</f>
@@ -3366,7 +3350,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C98" s="7">
         <v>110000000</v>
@@ -3379,7 +3363,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C99" s="7">
         <v>1800000</v>
@@ -3392,7 +3376,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C100" s="7">
         <v>547120000</v>
@@ -3405,7 +3389,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C101" s="7">
         <v>100000000</v>
@@ -3418,7 +3402,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C102" s="7">
         <v>447120000</v>
@@ -3431,7 +3415,7 @@
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C103" s="2">
         <f>C104+C113+C114+C120+C121+C122+C123+C124</f>
@@ -3444,7 +3428,7 @@
         <v>99</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C104" s="2">
         <v>332239129</v>
@@ -3456,7 +3440,7 @@
         <v>99</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C105" s="2">
         <v>500000</v>
@@ -3468,7 +3452,7 @@
         <v>99</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C106" s="2">
         <v>2000000</v>
@@ -3480,7 +3464,7 @@
         <v>99</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C107" s="2">
         <v>57486220</v>
@@ -3492,7 +3476,7 @@
         <v>99</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C108" s="2">
         <v>250000000</v>
@@ -3504,7 +3488,7 @@
         <v>99</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C109" s="2">
         <v>16196279</v>
@@ -3516,7 +3500,7 @@
         <v>99</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C110" s="2">
         <v>85000000</v>
@@ -3528,7 +3512,7 @@
         <v>99</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C111" s="2">
         <v>4684000</v>
@@ -3540,7 +3524,7 @@
         <v>99</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C112" s="2">
         <v>1287630</v>
@@ -3552,7 +3536,7 @@
         <v>99</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C113" s="2">
         <v>81280000</v>
@@ -3563,7 +3547,7 @@
         <v>99</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C114" s="2">
         <f>SUM(C115:C119)</f>
@@ -3575,7 +3559,7 @@
         <v>99</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C115" s="2">
         <v>1231900</v>
@@ -3586,7 +3570,7 @@
         <v>99</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C116" s="2">
         <v>10814050</v>
@@ -3597,7 +3581,7 @@
         <v>99</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C117" s="2">
         <v>3619500</v>
@@ -3608,7 +3592,7 @@
         <v>99</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C118" s="2">
         <v>1651000</v>
@@ -3619,7 +3603,7 @@
         <v>99</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C119" s="2">
         <v>1714500</v>
@@ -3630,7 +3614,7 @@
         <v>99</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="C120" s="2">
         <v>151050000</v>
@@ -3642,7 +3626,7 @@
         <v>99</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C121" s="2">
         <v>939800</v>
@@ -3653,7 +3637,7 @@
         <v>99</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C122" s="2">
         <v>2933060</v>
@@ -3664,7 +3648,7 @@
         <v>99</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C123" s="2">
         <v>4379450</v>
@@ -3675,7 +3659,7 @@
         <v>99</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="C124" s="2">
         <v>7200900</v>
@@ -3686,7 +3670,7 @@
         <v>99</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C125" s="5">
         <f>C126+C132+C135</f>
@@ -3699,7 +3683,7 @@
         <v>99</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C126" s="2">
         <f>C127+C128+C129+C130+C131</f>
@@ -3711,7 +3695,7 @@
         <v>99</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C127" s="2">
         <v>533000000</v>
@@ -3722,7 +3706,7 @@
         <v>99</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="C128" s="2">
         <v>170000000</v>
@@ -3733,7 +3717,7 @@
         <v>99</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C129" s="2">
         <v>45000000</v>
@@ -3744,7 +3728,7 @@
         <v>99</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="C130" s="2">
         <v>110000000</v>
@@ -3755,7 +3739,7 @@
         <v>99</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C131" s="2">
         <v>145588402</v>
@@ -3766,7 +3750,7 @@
         <v>99</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C132" s="2">
         <f>C133+C134</f>
@@ -3778,7 +3762,7 @@
         <v>99</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C133" s="2">
         <v>620000000</v>
@@ -3789,7 +3773,7 @@
         <v>99</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C134" s="2">
         <v>167400000</v>
@@ -3800,7 +3784,7 @@
         <v>99</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C135" s="2">
         <f>C136+C137+C138+C139+C140+C141+C142+C143</f>
@@ -3812,7 +3796,7 @@
         <v>99</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C136" s="2">
         <v>20000000</v>
@@ -3823,7 +3807,7 @@
         <v>99</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C137" s="2">
         <v>69000000</v>
@@ -3834,7 +3818,7 @@
         <v>99</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="C138" s="2">
         <v>325000000</v>
@@ -3845,7 +3829,7 @@
         <v>99</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C139" s="2">
         <v>173000000</v>
@@ -3856,7 +3840,7 @@
         <v>99</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="C140" s="2">
         <v>15000000</v>
@@ -3867,7 +3851,7 @@
         <v>99</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C141" s="2">
         <v>24000000</v>
@@ -3878,7 +3862,7 @@
         <v>99</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C142" s="2">
         <v>30000000</v>
@@ -3889,7 +3873,7 @@
         <v>99</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="C143" s="2">
         <v>171720000</v>
@@ -3900,7 +3884,7 @@
         <v>99</v>
       </c>
       <c r="B144" s="6" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C144" s="5">
         <f>C145+C148+C156</f>
@@ -3913,7 +3897,7 @@
         <v>99</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C145" s="13">
         <f>C146+C147</f>
@@ -3926,7 +3910,7 @@
         <v>99</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C146" s="14">
         <v>356000000</v>
@@ -3938,7 +3922,7 @@
         <v>99</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C147" s="13">
         <v>20000000</v>
@@ -3950,7 +3934,7 @@
         <v>99</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C148" s="14">
         <f>SUM(C149:C155)</f>
@@ -3965,7 +3949,7 @@
         <v>99</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C149" s="16">
         <v>500000</v>
@@ -3979,7 +3963,7 @@
         <v>99</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C150" s="16">
         <v>145000000</v>
@@ -3993,7 +3977,7 @@
         <v>99</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C151" s="17">
         <v>50000000</v>
@@ -4007,7 +3991,7 @@
         <v>99</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C152" s="16">
         <v>7000000</v>
@@ -4021,7 +4005,7 @@
         <v>99</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C153" s="16">
         <v>4500000</v>
@@ -4035,7 +4019,7 @@
         <v>99</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C154" s="16">
         <v>17000000</v>
@@ -4049,7 +4033,7 @@
         <v>99</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="C155" s="16">
         <v>16000000</v>
@@ -4063,7 +4047,7 @@
         <v>99</v>
       </c>
       <c r="B156" s="18" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C156" s="16">
         <f>C157+C158</f>
@@ -4078,7 +4062,7 @@
         <v>99</v>
       </c>
       <c r="B157" s="15" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C157" s="14">
         <v>400000000</v>
@@ -4092,7 +4076,7 @@
         <v>99</v>
       </c>
       <c r="B158" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="C158" s="2">
         <v>673100000</v>
@@ -4120,7 +4104,7 @@
   <dimension ref="A1:C56"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B61" sqref="B61"/>
+      <selection activeCell="B57" sqref="B57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4131,7 +4115,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4183,7 +4167,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="C6" s="28">
         <v>462309000</v>
@@ -4194,7 +4178,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C7" s="28">
         <v>5997600</v>
@@ -4205,7 +4189,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="C8" s="28">
         <v>11939410</v>
@@ -4216,7 +4200,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C9" s="28">
         <v>99559800</v>
@@ -4238,7 +4222,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="C11" s="2">
         <v>59121800</v>
@@ -4249,7 +4233,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C12" s="2">
         <v>270785550</v>
@@ -4260,7 +4244,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="C13" s="2">
         <v>15282000</v>
@@ -4271,7 +4255,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C14" s="2">
         <v>811600</v>
@@ -4282,7 +4266,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="C15" s="2">
         <v>119679000</v>
@@ -4304,7 +4288,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C17" s="2">
         <v>100443284</v>
@@ -4315,7 +4299,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="C18" s="2">
         <v>154589000</v>
@@ -4326,7 +4310,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C19" s="2">
         <v>53810320</v>
@@ -4337,7 +4321,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="C20" s="2">
         <v>137494427</v>
@@ -4458,7 +4442,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>378</v>
+        <v>368</v>
       </c>
       <c r="C31" s="2">
         <v>2285897273</v>
@@ -4469,7 +4453,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C32" s="2">
         <v>64986200</v>
@@ -4480,7 +4464,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C33" s="2">
         <v>91990000</v>
@@ -4491,7 +4475,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="2">
         <v>1440700000</v>
@@ -4502,7 +4486,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C35" s="2">
         <v>266600000</v>
@@ -4513,7 +4497,7 @@
         <v>99</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C36" s="2">
         <v>427400000</v>
@@ -4524,7 +4508,7 @@
         <v>99</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C37" s="2">
         <v>135000000</v>
@@ -4535,7 +4519,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C38" s="2">
         <v>500000000</v>
@@ -4546,7 +4530,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C39" s="2">
         <v>46700000</v>
@@ -4557,7 +4541,7 @@
         <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C40" s="2">
         <v>65000000</v>
@@ -4568,7 +4552,7 @@
         <v>99</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="2">
         <v>83098010</v>
@@ -4579,7 +4563,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C42" s="2">
         <v>379225063</v>
@@ -4590,7 +4574,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C43" s="2">
         <v>125498000</v>
@@ -4601,7 +4585,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C44" s="2">
         <v>95000000</v>
@@ -4612,7 +4596,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="C45" s="2">
         <v>5000000</v>
@@ -4623,7 +4607,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>379</v>
+        <v>369</v>
       </c>
       <c r="C46" s="2">
         <v>400000</v>
@@ -4634,7 +4618,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>380</v>
+        <v>370</v>
       </c>
       <c r="C47" s="2">
         <v>1310255998</v>
@@ -4645,7 +4629,7 @@
         <v>99</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>381</v>
+        <v>371</v>
       </c>
       <c r="C48" s="2">
         <v>968100000</v>
@@ -4656,7 +4640,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>382</v>
+        <v>372</v>
       </c>
       <c r="C49" s="2">
         <v>200000000</v>
@@ -4667,7 +4651,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>383</v>
+        <v>373</v>
       </c>
       <c r="C50" s="2">
         <v>142155998</v>
@@ -4678,7 +4662,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>384</v>
+        <v>374</v>
       </c>
       <c r="C51" s="2">
         <v>6712832403</v>
@@ -4689,7 +4673,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>385</v>
+        <v>375</v>
       </c>
       <c r="C52" s="2">
         <v>1994660000</v>
@@ -4700,7 +4684,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>386</v>
+        <v>376</v>
       </c>
       <c r="C53" s="2">
         <v>4718172403</v>
@@ -4711,7 +4695,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C54" s="2">
         <v>6712832403</v>
@@ -4730,8 +4714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{360EBD22-8A27-462E-8847-1D905C6EB368}">
   <dimension ref="A1:BG202"/>
   <sheetViews>
-    <sheetView topLeftCell="A198" workbookViewId="0">
-      <selection activeCell="C212" sqref="C212"/>
+    <sheetView topLeftCell="A48" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4783,7 +4767,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
@@ -4797,172 +4781,172 @@
         <v>1</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>314</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>315</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>316</v>
+      </c>
+      <c r="H2" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="I2" s="29" t="s">
+        <v>318</v>
+      </c>
+      <c r="J2" s="29" t="s">
+        <v>319</v>
+      </c>
+      <c r="K2" s="29" t="s">
+        <v>320</v>
+      </c>
+      <c r="L2" s="29" t="s">
+        <v>321</v>
+      </c>
+      <c r="M2" s="29" t="s">
+        <v>322</v>
+      </c>
+      <c r="N2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="S2" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="T2" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="U2" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="V2" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="W2" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="X2" s="29" t="s">
         <v>333</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="Y2" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="Z2" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="AA2" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="AB2" s="29" t="s">
         <v>337</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="AC2" s="29" t="s">
         <v>338</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="AD2" s="29" t="s">
         <v>339</v>
       </c>
-      <c r="U2" s="29" t="s">
+      <c r="AE2" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="AF2" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="AG2" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="AH2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="Y2" s="29" t="s">
+      <c r="AI2" s="29" t="s">
         <v>344</v>
       </c>
-      <c r="Z2" s="29" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="AA2" s="29" t="s">
+      <c r="AK2" s="29" t="s">
         <v>346</v>
       </c>
-      <c r="AB2" s="29" t="s">
+      <c r="AL2" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="AC2" s="29" t="s">
+      <c r="AM2" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AN2" s="29" t="s">
         <v>349</v>
       </c>
-      <c r="AE2" s="29" t="s">
+      <c r="AO2" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="AF2" s="29" t="s">
+      <c r="AP2" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AQ2" s="29" t="s">
         <v>352</v>
       </c>
-      <c r="AH2" s="29" t="s">
+      <c r="AR2" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="AI2" s="29" t="s">
+      <c r="AS2" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="AJ2" s="29" t="s">
+      <c r="AT2" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="AU2" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="AL2" s="29" t="s">
+      <c r="AV2" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="AM2" s="29" t="s">
+      <c r="AW2" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="AN2" s="29" t="s">
+      <c r="AX2" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="AO2" s="29" t="s">
+      <c r="AY2" s="29" t="s">
+        <v>317</v>
+      </c>
+      <c r="AZ2" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="AP2" s="29" t="s">
+      <c r="BA2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="AQ2" s="29" t="s">
+      <c r="BB2" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="AR2" s="29" t="s">
+      <c r="BC2" s="29" t="s">
         <v>363</v>
       </c>
-      <c r="AS2" s="29" t="s">
+      <c r="BD2" s="29" t="s">
         <v>364</v>
       </c>
-      <c r="AT2" s="29" t="s">
+      <c r="BE2" s="29" t="s">
         <v>365</v>
       </c>
-      <c r="AU2" s="29" t="s">
+      <c r="BF2" s="29" t="s">
         <v>366</v>
       </c>
-      <c r="AV2" s="29" t="s">
-        <v>367</v>
-      </c>
-      <c r="AW2" s="29" t="s">
-        <v>368</v>
-      </c>
-      <c r="AX2" s="29" t="s">
-        <v>369</v>
-      </c>
-      <c r="AY2" s="29" t="s">
-        <v>327</v>
-      </c>
-      <c r="AZ2" s="29" t="s">
-        <v>370</v>
-      </c>
-      <c r="BA2" s="29" t="s">
-        <v>371</v>
-      </c>
-      <c r="BB2" s="29" t="s">
-        <v>372</v>
-      </c>
-      <c r="BC2" s="29" t="s">
-        <v>373</v>
-      </c>
-      <c r="BD2" s="29" t="s">
-        <v>374</v>
-      </c>
-      <c r="BE2" s="29" t="s">
-        <v>375</v>
-      </c>
-      <c r="BF2" s="29" t="s">
-        <v>376</v>
-      </c>
       <c r="BG2" s="29" t="s">
-        <v>334</v>
+        <v>324</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
@@ -4970,7 +4954,7 @@
         <v>99</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="C3" s="32">
         <v>5103770263</v>
@@ -4981,7 +4965,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="C4" s="32">
         <v>222768231</v>
@@ -4992,7 +4976,7 @@
         <v>99</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
       <c r="C5" s="32">
         <v>189960800</v>
@@ -5003,7 +4987,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
       <c r="C6" s="32">
         <v>32807431</v>
@@ -5014,7 +4998,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
       <c r="C7" s="32">
         <v>2043364244</v>
@@ -5025,7 +5009,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="C8" s="32">
         <v>1732037214</v>
@@ -5036,7 +5020,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="C9" s="32">
         <v>16842828</v>
@@ -5047,7 +5031,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="C10" s="32">
         <v>294484202</v>
@@ -5058,7 +5042,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="C11" s="32">
         <v>640438866</v>
@@ -5069,7 +5053,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C12" s="32">
         <v>93243562</v>
@@ -5080,7 +5064,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>53</v>
+        <v>45</v>
       </c>
       <c r="C13" s="32">
         <v>79251341</v>
@@ -5091,7 +5075,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C14" s="32">
         <v>1000000</v>
@@ -5102,7 +5086,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
       <c r="C15" s="32">
         <v>12992221</v>
@@ -5113,7 +5097,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C16" s="32">
         <v>149693557</v>
@@ -5124,7 +5108,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C17" s="32">
         <v>125277036</v>
@@ -5135,7 +5119,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C18" s="32">
         <v>1734915</v>
@@ -5146,7 +5130,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="C19" s="32">
         <v>22681606</v>
@@ -5157,7 +5141,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C20" s="32">
         <v>104072380</v>
@@ -5168,7 +5152,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C21" s="32">
         <v>89039212</v>
@@ -5179,7 +5163,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C22" s="32">
         <v>578000</v>
@@ -5190,7 +5174,7 @@
         <v>99</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="C23" s="32">
         <v>14455168</v>
@@ -5201,7 +5185,7 @@
         <v>99</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C24" s="32">
         <v>149086199</v>
@@ -5212,7 +5196,7 @@
         <v>99</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C25" s="32">
         <v>124929241</v>
@@ -5223,7 +5207,7 @@
         <v>99</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C26" s="32">
         <v>1370000</v>
@@ -5234,7 +5218,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C27" s="32">
         <v>22786958</v>
@@ -5245,7 +5229,7 @@
         <v>99</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C28" s="32">
         <v>144343168</v>
@@ -5256,7 +5240,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C29" s="32">
         <v>121478024</v>
@@ -5267,7 +5251,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C30" s="32">
         <v>1441000</v>
@@ -5278,7 +5262,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C31" s="32">
         <v>21424144</v>
@@ -5289,7 +5273,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C32" s="32">
         <v>1326100000</v>
@@ -5300,7 +5284,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C33" s="32">
         <v>1120587200</v>
@@ -5311,7 +5295,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C34" s="32">
         <v>17088000</v>
@@ -5322,7 +5306,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C35" s="32">
         <v>188424800</v>
@@ -5333,7 +5317,7 @@
         <v>99</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C36" s="32">
         <v>42027890</v>
@@ -5344,7 +5328,7 @@
         <v>99</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C37" s="32">
         <v>34811556</v>
@@ -5355,7 +5339,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C38" s="32">
         <v>1310000</v>
@@ -5366,7 +5350,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C39" s="32">
         <v>5906334</v>
@@ -5377,7 +5361,7 @@
         <v>99</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C40" s="32">
         <v>300466210</v>
@@ -5388,7 +5372,7 @@
         <v>99</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C41" s="32">
         <v>247951691</v>
@@ -5399,7 +5383,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C42" s="32">
         <v>6335400</v>
@@ -5410,7 +5394,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C43" s="32">
         <v>46179119</v>
@@ -5421,7 +5405,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C44" s="32">
         <v>223227098</v>
@@ -5432,7 +5416,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C45" s="32">
         <v>188228592</v>
@@ -5443,7 +5427,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C46" s="32">
         <v>1250000</v>
@@ -5454,7 +5438,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C47" s="32">
         <v>33748506</v>
@@ -5465,7 +5449,7 @@
         <v>99</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C48" s="32">
         <v>305377724</v>
@@ -5476,7 +5460,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C49" s="32">
         <v>259300317</v>
@@ -5487,7 +5471,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C50" s="32">
         <v>250000</v>
@@ -5498,7 +5482,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C51" s="32">
         <v>45827407</v>
@@ -5509,7 +5493,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C52" s="32">
         <v>5554643775</v>
@@ -5520,7 +5504,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C53" s="32">
         <v>4603346824</v>
@@ -5531,7 +5515,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C54" s="33">
         <v>40477590</v>
@@ -5542,7 +5526,7 @@
         <v>99</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C55" s="33">
         <v>62775000</v>
@@ -5553,7 +5537,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C56" s="33">
         <v>3171066602</v>
@@ -5564,7 +5548,7 @@
         <v>99</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>97</v>
+        <v>382</v>
       </c>
       <c r="C57" s="33">
         <v>64100000</v>
@@ -5575,7 +5559,7 @@
         <v>99</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="C58" s="33">
         <v>1264927632</v>
@@ -5586,7 +5570,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C59" s="32">
         <v>365086335</v>
@@ -5597,7 +5581,7 @@
         <v>99</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C60" s="32">
         <v>36000000</v>
@@ -5608,7 +5592,7 @@
         <v>99</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C61" s="32">
         <v>47360000</v>
@@ -5619,7 +5603,7 @@
         <v>99</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="C62" s="32">
         <v>195455450</v>
@@ -5630,7 +5614,7 @@
         <v>99</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>223</v>
+        <v>383</v>
       </c>
       <c r="C63" s="32">
         <v>0</v>
@@ -5641,7 +5625,7 @@
         <v>99</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>224</v>
+        <v>214</v>
       </c>
       <c r="C64" s="32">
         <v>86270885</v>
@@ -5652,7 +5636,7 @@
         <v>99</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C65" s="32">
         <v>78107500</v>
@@ -5663,7 +5647,7 @@
         <v>99</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C66" s="32">
         <v>10205750</v>
@@ -5674,7 +5658,7 @@
         <v>99</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C67" s="32">
         <v>18945750</v>
@@ -5685,7 +5669,7 @@
         <v>99</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="C68" s="32">
         <v>14116750</v>
@@ -5696,7 +5680,7 @@
         <v>99</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C69" s="32">
         <v>15148150</v>
@@ -5707,7 +5691,7 @@
         <v>99</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="C70" s="32">
         <v>19691100</v>
@@ -5718,7 +5702,7 @@
         <v>99</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C71" s="32">
         <v>294000000</v>
@@ -5729,7 +5713,7 @@
         <v>99</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="C72" s="32">
         <v>13207980</v>
@@ -5740,7 +5724,7 @@
         <v>99</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C73" s="32">
         <v>103891480</v>
@@ -5751,7 +5735,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="C74" s="32">
         <v>40623646</v>
@@ -5762,7 +5746,7 @@
         <v>99</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="C75" s="32">
         <v>56380010</v>
@@ -5773,7 +5757,7 @@
         <v>99</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C76" s="32">
         <v>408568000</v>
@@ -5784,7 +5768,7 @@
         <v>99</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>225</v>
+        <v>215</v>
       </c>
       <c r="C77" s="32">
         <v>126544000</v>
@@ -5795,7 +5779,7 @@
         <v>99</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="C78" s="32">
         <v>35000000</v>
@@ -5806,7 +5790,7 @@
         <v>99</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="C79" s="32">
         <v>7824000</v>
@@ -5817,7 +5801,7 @@
         <v>99</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>228</v>
+        <v>218</v>
       </c>
       <c r="C80" s="32">
         <v>40000000</v>
@@ -5828,7 +5812,7 @@
         <v>99</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>229</v>
+        <v>219</v>
       </c>
       <c r="C81" s="32">
         <v>1000000</v>
@@ -5839,7 +5823,7 @@
         <v>99</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>230</v>
+        <v>220</v>
       </c>
       <c r="C82" s="32">
         <v>720000</v>
@@ -5850,7 +5834,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>231</v>
+        <v>221</v>
       </c>
       <c r="C83" s="32">
         <v>40000000</v>
@@ -5861,7 +5845,7 @@
         <v>99</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>232</v>
+        <v>222</v>
       </c>
       <c r="C84" s="32">
         <v>2000000</v>
@@ -5872,7 +5856,7 @@
         <v>99</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>233</v>
+        <v>223</v>
       </c>
       <c r="C85" s="32">
         <v>282024000</v>
@@ -5883,7 +5867,7 @@
         <v>99</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
       <c r="C86" s="32">
         <v>50000000</v>
@@ -5894,7 +5878,7 @@
         <v>99</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>235</v>
+        <v>225</v>
       </c>
       <c r="C87" s="32">
         <v>2000000</v>
@@ -5905,7 +5889,7 @@
         <v>99</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>236</v>
+        <v>226</v>
       </c>
       <c r="C88" s="32">
         <v>12000000</v>
@@ -5916,7 +5900,7 @@
         <v>99</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>237</v>
+        <v>227</v>
       </c>
       <c r="C89" s="32">
         <v>3000000</v>
@@ -5927,7 +5911,7 @@
         <v>99</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>238</v>
+        <v>228</v>
       </c>
       <c r="C90" s="32">
         <v>80000000</v>
@@ -5938,7 +5922,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>239</v>
+        <v>229</v>
       </c>
       <c r="C91" s="32">
         <v>22500000</v>
@@ -5949,7 +5933,7 @@
         <v>99</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>240</v>
+        <v>230</v>
       </c>
       <c r="C92" s="32">
         <v>8000000</v>
@@ -5960,7 +5944,7 @@
         <v>99</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C93" s="32">
         <v>500000</v>
@@ -5971,7 +5955,7 @@
         <v>99</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>242</v>
+        <v>232</v>
       </c>
       <c r="C94" s="32">
         <v>22500000</v>
@@ -5982,7 +5966,7 @@
         <v>99</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>243</v>
+        <v>233</v>
       </c>
       <c r="C95" s="32">
         <v>4250000</v>
@@ -5993,7 +5977,7 @@
         <v>99</v>
       </c>
       <c r="B96" s="31" t="s">
-        <v>244</v>
+        <v>234</v>
       </c>
       <c r="C96" s="32">
         <v>1000000</v>
@@ -6004,7 +5988,7 @@
         <v>99</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C97" s="32">
         <v>10000000</v>
@@ -6015,7 +5999,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>246</v>
+        <v>236</v>
       </c>
       <c r="C98" s="32">
         <v>66274000</v>
@@ -6026,7 +6010,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="C99" s="32">
         <v>2706803035</v>
@@ -6037,7 +6021,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>247</v>
+        <v>237</v>
       </c>
       <c r="C100" s="32">
         <v>743201757</v>
@@ -6048,7 +6032,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>248</v>
+        <v>238</v>
       </c>
       <c r="C101" s="32">
         <v>41800000</v>
@@ -6059,7 +6043,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>249</v>
+        <v>239</v>
       </c>
       <c r="C102" s="32">
         <v>40000000</v>
@@ -6070,7 +6054,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>250</v>
+        <v>240</v>
       </c>
       <c r="C103" s="32">
         <v>1800000</v>
@@ -6081,7 +6065,7 @@
         <v>99</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>251</v>
+        <v>241</v>
       </c>
       <c r="C104" s="32">
         <v>874501278</v>
@@ -6092,7 +6076,7 @@
         <v>99</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>252</v>
+        <v>242</v>
       </c>
       <c r="C105" s="32">
         <v>40000000</v>
@@ -6103,7 +6087,7 @@
         <v>99</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>253</v>
+        <v>243</v>
       </c>
       <c r="C106" s="32">
         <v>67100000</v>
@@ -6114,7 +6098,7 @@
         <v>99</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>254</v>
+        <v>244</v>
       </c>
       <c r="C107" s="32">
         <v>17000000</v>
@@ -6125,7 +6109,7 @@
         <v>99</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>255</v>
+        <v>245</v>
       </c>
       <c r="C108" s="32">
         <v>2400000</v>
@@ -6136,7 +6120,7 @@
         <v>99</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>256</v>
+        <v>246</v>
       </c>
       <c r="C109" s="32">
         <v>32000000</v>
@@ -6147,7 +6131,7 @@
         <v>99</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>257</v>
+        <v>247</v>
       </c>
       <c r="C110" s="32">
         <v>2500000</v>
@@ -6158,7 +6142,7 @@
         <v>99</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="C111" s="32">
         <v>6000000</v>
@@ -6169,7 +6153,7 @@
         <v>99</v>
       </c>
       <c r="B112" s="31" t="s">
-        <v>259</v>
+        <v>249</v>
       </c>
       <c r="C112" s="32">
         <v>2100000</v>
@@ -6180,7 +6164,7 @@
         <v>99</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>260</v>
+        <v>250</v>
       </c>
       <c r="C113" s="32">
         <v>3000000</v>
@@ -6191,7 +6175,7 @@
         <v>99</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>261</v>
+        <v>251</v>
       </c>
       <c r="C114" s="32">
         <v>100000</v>
@@ -6202,7 +6186,7 @@
         <v>99</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>262</v>
+        <v>252</v>
       </c>
       <c r="C115" s="32">
         <v>2000000</v>
@@ -6213,7 +6197,7 @@
         <v>99</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>263</v>
+        <v>253</v>
       </c>
       <c r="C116" s="32">
         <v>10500000</v>
@@ -6224,7 +6208,7 @@
         <v>99</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>264</v>
+        <v>254</v>
       </c>
       <c r="C117" s="32">
         <v>500000</v>
@@ -6235,7 +6219,7 @@
         <v>99</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>265</v>
+        <v>255</v>
       </c>
       <c r="C118" s="32">
         <v>500000</v>
@@ -6246,7 +6230,7 @@
         <v>99</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>266</v>
+        <v>256</v>
       </c>
       <c r="C119" s="32">
         <v>500000</v>
@@ -6257,7 +6241,7 @@
         <v>99</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>267</v>
+        <v>257</v>
       </c>
       <c r="C120" s="32">
         <v>500000</v>
@@ -6268,7 +6252,7 @@
         <v>99</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>268</v>
+        <v>258</v>
       </c>
       <c r="C121" s="32">
         <v>500000</v>
@@ -6279,7 +6263,7 @@
         <v>99</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>269</v>
+        <v>259</v>
       </c>
       <c r="C122" s="32">
         <v>500000</v>
@@ -6290,7 +6274,7 @@
         <v>99</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>270</v>
+        <v>260</v>
       </c>
       <c r="C123" s="32">
         <v>4000000</v>
@@ -6301,7 +6285,7 @@
         <v>99</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>271</v>
+        <v>261</v>
       </c>
       <c r="C124" s="32">
         <v>1000000</v>
@@ -6312,7 +6296,7 @@
         <v>99</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>272</v>
+        <v>262</v>
       </c>
       <c r="C125" s="32">
         <v>2000000</v>
@@ -6323,7 +6307,7 @@
         <v>99</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>273</v>
+        <v>263</v>
       </c>
       <c r="C126" s="32">
         <v>500000</v>
@@ -6334,7 +6318,7 @@
         <v>99</v>
       </c>
       <c r="B127" s="31" t="s">
-        <v>274</v>
+        <v>264</v>
       </c>
       <c r="C127" s="32">
         <v>17000000</v>
@@ -6345,7 +6329,7 @@
         <v>99</v>
       </c>
       <c r="B128" s="31" t="s">
-        <v>275</v>
+        <v>265</v>
       </c>
       <c r="C128" s="32">
         <v>739901278</v>
@@ -6356,7 +6340,7 @@
         <v>99</v>
       </c>
       <c r="B129" s="31" t="s">
-        <v>276</v>
+        <v>266</v>
       </c>
       <c r="C129" s="32">
         <v>211901278</v>
@@ -6367,7 +6351,7 @@
         <v>99</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>277</v>
+        <v>267</v>
       </c>
       <c r="C130" s="2">
         <v>528000000</v>
@@ -6378,7 +6362,7 @@
         <v>99</v>
       </c>
       <c r="B131" s="31" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="C131" s="32">
         <v>1047300000</v>
@@ -6389,7 +6373,7 @@
         <v>99</v>
       </c>
       <c r="B132" s="31" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C132" s="32">
         <v>100000000</v>
@@ -6400,7 +6384,7 @@
         <v>99</v>
       </c>
       <c r="B133" s="31" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C133" s="32">
         <v>947300000</v>
@@ -6411,7 +6395,7 @@
         <v>99</v>
       </c>
       <c r="B134" s="31" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C134" s="2">
         <v>1301841058</v>
@@ -6422,7 +6406,7 @@
         <v>99</v>
       </c>
       <c r="B135" s="31" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C135" s="2">
         <v>1081323148</v>
@@ -6433,7 +6417,7 @@
         <v>99</v>
       </c>
       <c r="B136" s="31" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C136" s="2">
         <v>1287400</v>
@@ -6444,7 +6428,7 @@
         <v>99</v>
       </c>
       <c r="B137" s="31" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C137" s="2">
         <v>2000000</v>
@@ -6455,7 +6439,7 @@
         <v>99</v>
       </c>
       <c r="B138" s="31" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C138" s="2">
         <v>333345000</v>
@@ -6466,7 +6450,7 @@
         <v>99</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="C139" s="2">
         <v>653800000</v>
@@ -6477,7 +6461,7 @@
         <v>99</v>
       </c>
       <c r="B140" s="31" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C140" s="2">
         <v>90890748</v>
@@ -6488,7 +6472,7 @@
         <v>99</v>
       </c>
       <c r="B141" s="31" t="s">
-        <v>278</v>
+        <v>268</v>
       </c>
       <c r="C141" s="2">
         <v>5224780</v>
@@ -6499,7 +6483,7 @@
         <v>99</v>
       </c>
       <c r="B142" s="31" t="s">
-        <v>279</v>
+        <v>269</v>
       </c>
       <c r="C142" s="32">
         <v>81280000</v>
@@ -6510,7 +6494,7 @@
         <v>99</v>
       </c>
       <c r="B143" s="31" t="s">
-        <v>280</v>
+        <v>270</v>
       </c>
       <c r="C143" s="32">
         <v>16192500</v>
@@ -6521,7 +6505,7 @@
         <v>99</v>
       </c>
       <c r="B144" s="31" t="s">
-        <v>281</v>
+        <v>271</v>
       </c>
       <c r="C144" s="32">
         <v>94791110</v>
@@ -6532,7 +6516,7 @@
         <v>99</v>
       </c>
       <c r="B145" s="31" t="s">
-        <v>282</v>
+        <v>272</v>
       </c>
       <c r="C145" s="32">
         <v>811685</v>
@@ -6543,7 +6527,7 @@
         <v>99</v>
       </c>
       <c r="B146" s="31" t="s">
-        <v>283</v>
+        <v>273</v>
       </c>
       <c r="C146" s="32">
         <v>2325388</v>
@@ -6554,7 +6538,7 @@
         <v>99</v>
       </c>
       <c r="B147" s="31" t="s">
-        <v>284</v>
+        <v>274</v>
       </c>
       <c r="C147" s="32">
         <v>16946047</v>
@@ -6565,7 +6549,7 @@
         <v>99</v>
       </c>
       <c r="B148" s="31" t="s">
-        <v>285</v>
+        <v>275</v>
       </c>
       <c r="C148" s="32">
         <v>2946400</v>
@@ -6576,7 +6560,7 @@
         <v>99</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C149" s="2">
         <v>3585732832</v>
@@ -6587,7 +6571,7 @@
         <v>99</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="C150" s="2">
         <v>330962000</v>
@@ -6598,7 +6582,7 @@
         <v>99</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>286</v>
+        <v>276</v>
       </c>
       <c r="C151" s="2">
         <v>65000000</v>
@@ -6609,7 +6593,7 @@
         <v>99</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>287</v>
+        <v>277</v>
       </c>
       <c r="C152" s="2">
         <v>100000000</v>
@@ -6620,7 +6604,7 @@
         <v>99</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>288</v>
+        <v>278</v>
       </c>
       <c r="C153" s="2">
         <v>25000000</v>
@@ -6631,7 +6615,7 @@
         <v>99</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>289</v>
+        <v>279</v>
       </c>
       <c r="C154" s="2">
         <v>70600000</v>
@@ -6642,7 +6626,7 @@
         <v>99</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C155" s="2">
         <v>70362000</v>
@@ -6653,7 +6637,7 @@
         <v>99</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="C156" s="2">
         <v>796290000</v>
@@ -6664,7 +6648,7 @@
         <v>99</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C157" s="2">
         <v>613000000</v>
@@ -6675,7 +6659,7 @@
         <v>99</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>290</v>
+        <v>280</v>
       </c>
       <c r="C158" s="2">
         <v>5000000</v>
@@ -6686,7 +6670,7 @@
         <v>99</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>291</v>
+        <v>281</v>
       </c>
       <c r="C159" s="2">
         <v>9000000</v>
@@ -6697,7 +6681,7 @@
         <v>99</v>
       </c>
       <c r="B160" s="31" t="s">
-        <v>292</v>
+        <v>282</v>
       </c>
       <c r="C160" s="2">
         <v>169290000</v>
@@ -6708,7 +6692,7 @@
         <v>99</v>
       </c>
       <c r="B161" s="31" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C161" s="2">
         <v>648063647</v>
@@ -6719,7 +6703,7 @@
         <v>99</v>
       </c>
       <c r="B162" s="31" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C162" s="2">
         <v>20000000</v>
@@ -6730,7 +6714,7 @@
         <v>99</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C163" s="2">
         <v>20000000</v>
@@ -6741,7 +6725,7 @@
         <v>99</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>293</v>
+        <v>283</v>
       </c>
       <c r="C164" s="2">
         <v>120000000</v>
@@ -6752,7 +6736,7 @@
         <v>99</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>294</v>
+        <v>284</v>
       </c>
       <c r="C165" s="2">
         <v>60000000</v>
@@ -6763,7 +6747,7 @@
         <v>99</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>295</v>
+        <v>285</v>
       </c>
       <c r="C166" s="2">
         <v>265000000</v>
@@ -6774,7 +6758,7 @@
         <v>99</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>296</v>
+        <v>286</v>
       </c>
       <c r="C167" s="2">
         <v>110000000</v>
@@ -6785,7 +6769,7 @@
         <v>99</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>297</v>
+        <v>287</v>
       </c>
       <c r="C168" s="2">
         <v>19000000</v>
@@ -6796,7 +6780,7 @@
         <v>99</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>298</v>
+        <v>288</v>
       </c>
       <c r="C169" s="2">
         <v>34063647</v>
@@ -6807,7 +6791,7 @@
         <v>99</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>299</v>
+        <v>289</v>
       </c>
       <c r="C170" s="2">
         <v>1292000000</v>
@@ -6818,7 +6802,7 @@
         <v>99</v>
       </c>
       <c r="B171" s="31" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C171" s="2">
         <v>510000000</v>
@@ -6829,7 +6813,7 @@
         <v>99</v>
       </c>
       <c r="B172" s="31" t="s">
-        <v>301</v>
+        <v>291</v>
       </c>
       <c r="C172" s="2">
         <v>50000000</v>
@@ -6840,7 +6824,7 @@
         <v>99</v>
       </c>
       <c r="B173" s="31" t="s">
-        <v>302</v>
+        <v>292</v>
       </c>
       <c r="C173" s="2">
         <v>6000000</v>
@@ -6851,7 +6835,7 @@
         <v>99</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>303</v>
+        <v>293</v>
       </c>
       <c r="C174" s="2">
         <v>5000000</v>
@@ -6862,7 +6846,7 @@
         <v>99</v>
       </c>
       <c r="B175" s="31" t="s">
-        <v>304</v>
+        <v>294</v>
       </c>
       <c r="C175" s="2">
         <v>15000000</v>
@@ -6873,7 +6857,7 @@
         <v>99</v>
       </c>
       <c r="B176" s="31" t="s">
-        <v>305</v>
+        <v>295</v>
       </c>
       <c r="C176" s="2">
         <v>46000000</v>
@@ -6884,7 +6868,7 @@
         <v>99</v>
       </c>
       <c r="B177" s="31" t="s">
-        <v>306</v>
+        <v>296</v>
       </c>
       <c r="C177" s="2">
         <v>400000000</v>
@@ -6895,7 +6879,7 @@
         <v>99</v>
       </c>
       <c r="B178" s="31" t="s">
-        <v>307</v>
+        <v>297</v>
       </c>
       <c r="C178" s="2">
         <v>5000000</v>
@@ -6906,7 +6890,7 @@
         <v>99</v>
       </c>
       <c r="B179" s="31" t="s">
-        <v>308</v>
+        <v>298</v>
       </c>
       <c r="C179" s="2">
         <v>30000000</v>
@@ -6917,7 +6901,7 @@
         <v>99</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>309</v>
+        <v>299</v>
       </c>
       <c r="C180" s="2">
         <v>50000000</v>
@@ -6928,7 +6912,7 @@
         <v>99</v>
       </c>
       <c r="B181" s="31" t="s">
-        <v>310</v>
+        <v>300</v>
       </c>
       <c r="C181" s="2">
         <v>15000000</v>
@@ -6939,7 +6923,7 @@
         <v>99</v>
       </c>
       <c r="B182" s="31" t="s">
-        <v>311</v>
+        <v>301</v>
       </c>
       <c r="C182" s="2">
         <v>160000000</v>
@@ -6950,7 +6934,7 @@
         <v>99</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>312</v>
+        <v>302</v>
       </c>
       <c r="C183" s="2">
         <v>518417185</v>
@@ -6961,7 +6945,7 @@
         <v>99</v>
       </c>
       <c r="B184" s="31" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C184" s="2">
         <v>812243942</v>
@@ -6972,7 +6956,7 @@
         <v>99</v>
       </c>
       <c r="B185" s="31" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="C185" s="2">
         <v>355500000</v>
@@ -6983,7 +6967,7 @@
         <v>99</v>
       </c>
       <c r="B186" s="31" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C186" s="2">
         <v>345500000</v>
@@ -6994,7 +6978,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="31" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="C187" s="2">
         <v>10000000</v>
@@ -7005,7 +6989,7 @@
         <v>99</v>
       </c>
       <c r="B188" s="31" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C188" s="2">
         <v>226743942</v>
@@ -7016,7 +7000,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="31" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C189" s="34">
         <v>500000</v>
@@ -7027,7 +7011,7 @@
         <v>99</v>
       </c>
       <c r="B190" s="31" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C190" s="34">
         <v>145000000</v>
@@ -7038,7 +7022,7 @@
         <v>99</v>
       </c>
       <c r="B191" s="31" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C191" s="35">
         <v>30000000</v>
@@ -7049,7 +7033,7 @@
         <v>99</v>
       </c>
       <c r="B192" s="31" t="s">
-        <v>313</v>
+        <v>303</v>
       </c>
       <c r="C192" s="34">
         <v>5243942</v>
@@ -7060,7 +7044,7 @@
         <v>99</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>314</v>
+        <v>304</v>
       </c>
       <c r="C193" s="34">
         <v>15000000</v>
@@ -7071,7 +7055,7 @@
         <v>99</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>315</v>
+        <v>305</v>
       </c>
       <c r="C194" s="34">
         <v>10000000</v>
@@ -7082,7 +7066,7 @@
         <v>99</v>
       </c>
       <c r="B195" s="31" t="s">
-        <v>316</v>
+        <v>306</v>
       </c>
       <c r="C195" s="34">
         <v>5000000</v>
@@ -7093,7 +7077,7 @@
         <v>99</v>
       </c>
       <c r="B196" s="31" t="s">
-        <v>317</v>
+        <v>307</v>
       </c>
       <c r="C196" s="34">
         <v>5000000</v>
@@ -7104,7 +7088,7 @@
         <v>99</v>
       </c>
       <c r="B197" s="31" t="s">
-        <v>318</v>
+        <v>308</v>
       </c>
       <c r="C197" s="34">
         <v>3000000</v>
@@ -7115,7 +7099,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="31" t="s">
-        <v>319</v>
+        <v>309</v>
       </c>
       <c r="C198" s="34">
         <v>8000000</v>
@@ -7126,7 +7110,7 @@
         <v>99</v>
       </c>
       <c r="B199" s="31" t="s">
-        <v>320</v>
+        <v>310</v>
       </c>
       <c r="C199" s="34">
         <v>30000000</v>
@@ -7137,7 +7121,7 @@
         <v>99</v>
       </c>
       <c r="B200" s="31" t="s">
-        <v>321</v>
+        <v>311</v>
       </c>
       <c r="C200" s="34">
         <v>30000000</v>
@@ -7148,7 +7132,7 @@
         <v>99</v>
       </c>
       <c r="B201" s="31" t="s">
-        <v>322</v>
+        <v>312</v>
       </c>
       <c r="C201" s="34">
         <v>200000000</v>
@@ -7159,7 +7143,7 @@
         <v>99</v>
       </c>
       <c r="B202" t="s">
-        <v>377</v>
+        <v>367</v>
       </c>
       <c r="C202" s="2">
         <v>19473602905</v>

</xml_diff>

<commit_message>
added new budget and config
</commit_message>
<xml_diff>
--- a/input/budget.xlsx
+++ b/input/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4784027176d9b30c/_KMONITOR/_KÖKÖ/TERÉZVÁROS_KÖKÖ/2021_budget_config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1020" documentId="8_{E24534E0-E60B-4E45-949D-D5E79B4883FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{97C4DC14-F2C5-4E89-B6D7-4254112EA5D8}"/>
+  <xr:revisionPtr revIDLastSave="1029" documentId="8_{E24534E0-E60B-4E45-949D-D5E79B4883FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{581F29AE-9E7C-4200-89DA-2A6F51B3F210}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{501F2212-62D4-412E-9A6C-EB2F87D26B78}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{501F2212-62D4-412E-9A6C-EB2F87D26B78}"/>
   </bookViews>
   <sheets>
     <sheet name="2020 BEVÉTEL" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="517" uniqueCount="384">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="382">
   <si>
     <t>Megnevezés</t>
   </si>
@@ -140,9 +140,6 @@
     <t>Kamatbevételek (B37)</t>
   </si>
   <si>
-    <t>Finanszírozási többlet (maradvány) (FT1)</t>
-  </si>
-  <si>
     <t>Személyi juttatások és járulékok (K1)</t>
   </si>
   <si>
@@ -362,12 +359,6 @@
     <t>Egyéb működési célú kiadások  (K4)</t>
   </si>
   <si>
-    <t>Önkormányzat egyéb működési célú kiadásai (K41)</t>
-  </si>
-  <si>
-    <t>Elvonások és befizetések (K4101)</t>
-  </si>
-  <si>
     <t>Egyéb működési célú támogatás államháztartáson kívülre (K42)</t>
   </si>
   <si>
@@ -662,9 +653,6 @@
     <t>Egyéb működési bevételek (B38)</t>
   </si>
   <si>
-    <t>Finanszírozási többlet (maradvány, értékpapírok beváltása) (FT1)</t>
-  </si>
-  <si>
     <t>2021 KIADÁS</t>
   </si>
   <si>
@@ -1188,6 +1176,12 @@
   </si>
   <si>
     <t>Kiküldetés (K2204)</t>
+  </si>
+  <si>
+    <t>Finanszírozási bevétel - maradvány, értékpapírok beváltása (FT1)</t>
+  </si>
+  <si>
+    <t>Finanszírozási bevétel - maradvány (FT1)</t>
   </si>
 </sst>
 </file>
@@ -1652,8 +1646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96FAB4C5-B3A4-426F-A8BC-E577AEC02B08}">
   <dimension ref="A1:Q40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1872,7 +1866,7 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C18" s="2">
         <v>3779214700</v>
@@ -2040,7 +2034,7 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C33" s="2">
         <v>400000</v>
@@ -2051,7 +2045,7 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="C34" s="2">
         <v>1060817431</v>
@@ -2062,7 +2056,7 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="C35" s="2">
         <v>200000000</v>
@@ -2073,7 +2067,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="C36" s="2">
         <v>710636000</v>
@@ -2084,7 +2078,7 @@
         <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C37" s="2">
         <v>150181431</v>
@@ -2095,7 +2089,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="C38" s="2">
         <v>2826252158</v>
@@ -2106,7 +2100,7 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
+        <v>381</v>
       </c>
       <c r="C39" s="2">
         <v>2826252158</v>
@@ -2127,10 +2121,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C76BAFE8-6BF8-4E8A-B864-E53778D2F9B3}">
-  <dimension ref="A1:F161"/>
+  <dimension ref="A1:F160"/>
   <sheetViews>
-    <sheetView topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="D52" sqref="D52"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="B77" sqref="B77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2168,10 +2162,9 @@
         <v>99</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="7">
-        <f>C4+C7+C11+C32+C36+C40+C44+C48</f>
         <v>4487046138</v>
       </c>
       <c r="E3" s="25"/>
@@ -2182,10 +2175,9 @@
         <v>99</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="7">
-        <f>SUM(C5:C6)</f>
         <v>259668182</v>
       </c>
       <c r="E4" s="25"/>
@@ -2195,7 +2187,7 @@
         <v>99</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="7">
         <v>217908168</v>
@@ -2207,7 +2199,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="7">
         <v>41760014</v>
@@ -2219,10 +2211,9 @@
         <v>99</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="7">
-        <f>SUM(C8:C10)</f>
         <v>1871508962</v>
       </c>
       <c r="E7" s="25"/>
@@ -2232,7 +2223,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="7">
         <v>1538081462</v>
@@ -2244,7 +2235,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="7">
         <v>21615392</v>
@@ -2256,7 +2247,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="7">
         <v>311812108</v>
@@ -2268,10 +2259,9 @@
         <v>99</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="7">
-        <f>C12+C16+C20+C24+C28</f>
         <v>630500054</v>
       </c>
       <c r="E11" s="25"/>
@@ -2281,10 +2271,9 @@
         <v>99</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="7">
-        <f>SUM(C13:C15)</f>
         <v>93616705</v>
       </c>
       <c r="E12" s="25"/>
@@ -2294,7 +2283,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="7">
         <v>77428849</v>
@@ -2306,7 +2295,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="7">
         <v>900000</v>
@@ -2318,7 +2307,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="7">
         <v>15287856</v>
@@ -2330,10 +2319,9 @@
         <v>99</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="7">
-        <f>SUM(C17:C19)</f>
         <v>147266114</v>
       </c>
       <c r="E16" s="25"/>
@@ -2343,7 +2331,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="7">
         <v>117364155</v>
@@ -2355,7 +2343,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="7">
         <v>3977000</v>
@@ -2367,7 +2355,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="7">
         <v>25924959</v>
@@ -2379,10 +2367,9 @@
         <v>99</v>
       </c>
       <c r="B20" s="6" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="7">
-        <f>SUM(C21:C23)</f>
         <v>101268754</v>
       </c>
       <c r="E20" s="25"/>
@@ -2392,7 +2379,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="7">
         <v>83957303</v>
@@ -2404,7 +2391,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="7">
         <v>770000</v>
@@ -2416,7 +2403,7 @@
         <v>99</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="7">
         <v>16541451</v>
@@ -2428,10 +2415,9 @@
         <v>99</v>
       </c>
       <c r="B24" s="6" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="7">
-        <f>SUM(C25:C27)</f>
         <v>147733184</v>
       </c>
       <c r="E24" s="25"/>
@@ -2441,7 +2427,7 @@
         <v>99</v>
       </c>
       <c r="B25" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="7">
         <v>119592948</v>
@@ -2453,7 +2439,7 @@
         <v>99</v>
       </c>
       <c r="B26" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="7">
         <v>1870000</v>
@@ -2465,7 +2451,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="7">
         <v>26270236</v>
@@ -2477,10 +2463,9 @@
         <v>99</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="7">
-        <f>SUM(C29:C31)</f>
         <v>140615297</v>
       </c>
       <c r="E28" s="25"/>
@@ -2490,7 +2475,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="7">
         <v>113855057</v>
@@ -2502,7 +2487,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="7">
         <v>2490000</v>
@@ -2514,7 +2499,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="7">
         <v>24270240</v>
@@ -2526,10 +2511,9 @@
         <v>99</v>
       </c>
       <c r="B32" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="7">
-        <f>SUM(C33:C35)</f>
         <v>896843000</v>
       </c>
       <c r="E32" s="25"/>
@@ -2539,7 +2523,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="6" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="7">
         <v>673123300</v>
@@ -2551,7 +2535,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="7">
         <v>82875200</v>
@@ -2563,7 +2547,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="7">
         <v>140844500</v>
@@ -2575,10 +2559,9 @@
         <v>99</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="7">
-        <f>SUM(C37:C39)</f>
         <v>45451049</v>
       </c>
       <c r="E36" s="25"/>
@@ -2588,7 +2571,7 @@
         <v>99</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="7">
         <v>36680461</v>
@@ -2600,7 +2583,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="7">
         <v>1310000</v>
@@ -2612,7 +2595,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="7">
         <v>7460588</v>
@@ -2624,10 +2607,9 @@
         <v>99</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="7">
-        <f>SUM(C41:C43)</f>
         <v>296456264</v>
       </c>
       <c r="E40" s="25"/>
@@ -2637,7 +2619,7 @@
         <v>99</v>
       </c>
       <c r="B41" s="6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="7">
         <v>237656627</v>
@@ -2649,7 +2631,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="7">
         <v>5764400</v>
@@ -2661,7 +2643,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="7">
         <v>53035237</v>
@@ -2673,10 +2655,9 @@
         <v>99</v>
       </c>
       <c r="B44" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="7">
-        <f>SUM(C45:C47)</f>
         <v>216655982</v>
       </c>
       <c r="E44" s="25"/>
@@ -2686,7 +2667,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" s="7">
         <v>177302965</v>
@@ -2698,7 +2679,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="7">
         <v>1250000</v>
@@ -2710,7 +2691,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="7">
         <v>38103017</v>
@@ -2722,10 +2703,9 @@
         <v>99</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="7">
-        <f>SUM(C49:C51)</f>
         <v>269962645</v>
       </c>
       <c r="E48" s="25"/>
@@ -2735,7 +2715,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="7">
         <v>222010984</v>
@@ -2747,7 +2727,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="7">
         <v>250000</v>
@@ -2759,7 +2739,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="7">
         <v>47701661</v>
@@ -2771,10 +2751,9 @@
         <v>99</v>
       </c>
       <c r="B52" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C52" s="7">
-        <f>C53+C59+C60+C66+C67+C68+C69+C70</f>
         <v>6219752943</v>
       </c>
       <c r="E52" s="25"/>
@@ -2784,7 +2763,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="7">
         <v>5287267089</v>
@@ -2796,7 +2775,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" s="23">
         <v>29970956</v>
@@ -2808,7 +2787,7 @@
         <v>99</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="23">
         <v>58065000</v>
@@ -2820,7 +2799,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="23">
         <v>3451726392</v>
@@ -2832,7 +2811,7 @@
         <v>99</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C57" s="23">
         <v>91132500</v>
@@ -2844,7 +2823,7 @@
         <v>99</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C58" s="23">
         <v>1656372241</v>
@@ -2856,7 +2835,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C59" s="7">
         <v>370941077</v>
@@ -2868,10 +2847,9 @@
         <v>99</v>
       </c>
       <c r="B60" s="6" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C60" s="7">
-        <f>SUM(C61:C65)</f>
         <v>80168400</v>
       </c>
       <c r="E60" s="25"/>
@@ -2881,7 +2859,7 @@
         <v>99</v>
       </c>
       <c r="B61" s="6" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C61" s="7">
         <v>10881300</v>
@@ -2893,7 +2871,7 @@
         <v>99</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C62" s="7">
         <v>19492650</v>
@@ -2905,7 +2883,7 @@
         <v>99</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" s="7">
         <v>15397500</v>
@@ -2917,7 +2895,7 @@
         <v>99</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C64" s="7">
         <v>15516450</v>
@@ -2929,7 +2907,7 @@
         <v>99</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C65" s="7">
         <v>18880500</v>
@@ -2941,7 +2919,7 @@
         <v>99</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C66" s="7">
         <v>269407000</v>
@@ -2953,7 +2931,7 @@
         <v>99</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C67" s="7">
         <v>13312063</v>
@@ -2965,7 +2943,7 @@
         <v>99</v>
       </c>
       <c r="B68" s="6" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C68" s="7">
         <v>96503877</v>
@@ -2977,7 +2955,7 @@
         <v>99</v>
       </c>
       <c r="B69" s="6" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C69" s="7">
         <v>40761893</v>
@@ -2989,7 +2967,7 @@
         <v>99</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C70" s="7">
         <v>61391544</v>
@@ -3001,10 +2979,9 @@
         <v>99</v>
       </c>
       <c r="B71" s="6" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C71" s="7">
-        <f>C72+C73+C74+C75</f>
         <v>377546400</v>
       </c>
       <c r="E71" s="25"/>
@@ -3014,7 +2991,7 @@
         <v>99</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C72" s="7">
         <v>374096400</v>
@@ -3026,7 +3003,7 @@
         <v>99</v>
       </c>
       <c r="B73" s="6" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C73" s="7">
         <v>120000</v>
@@ -3038,7 +3015,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="C74" s="7">
         <v>130000</v>
@@ -3050,7 +3027,7 @@
         <v>99</v>
       </c>
       <c r="B75" s="6" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C75" s="7">
         <v>3200000</v>
@@ -3062,10 +3039,9 @@
         <v>99</v>
       </c>
       <c r="B76" s="6" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C76" s="7">
-        <f>C77+C79+C97+C100</f>
         <v>1495045857</v>
       </c>
       <c r="E76" s="25"/>
@@ -3074,11 +3050,10 @@
       <c r="A77" s="9">
         <v>99</v>
       </c>
-      <c r="B77" s="6" t="s">
-        <v>108</v>
+      <c r="B77" s="31" t="s">
+        <v>233</v>
       </c>
       <c r="C77" s="7">
-        <f>C78</f>
         <v>38602000</v>
       </c>
       <c r="E77" s="25"/>
@@ -3088,10 +3063,10 @@
         <v>99</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="C78" s="7">
-        <v>38602000</v>
+        <v>797523857</v>
       </c>
       <c r="E78" s="25"/>
     </row>
@@ -3100,36 +3075,36 @@
         <v>99</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C79" s="7">
-        <f>C80+C81+C82+C83+C93</f>
-        <v>797523857</v>
-      </c>
+        <v>40000000</v>
+      </c>
+      <c r="D79" s="8"/>
       <c r="E79" s="25"/>
     </row>
-    <row r="80" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:5" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="9">
         <v>99</v>
       </c>
       <c r="B80" s="6" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C80" s="7">
-        <v>40000000</v>
+        <v>17000000</v>
       </c>
       <c r="D80" s="8"/>
       <c r="E80" s="25"/>
     </row>
-    <row r="81" spans="1:5" s="6" customFormat="1" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A81" s="9">
         <v>99</v>
       </c>
       <c r="B81" s="6" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C81" s="7">
-        <v>17000000</v>
+        <v>6000000</v>
       </c>
       <c r="D81" s="8"/>
       <c r="E81" s="25"/>
@@ -3139,34 +3114,33 @@
         <v>99</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C82" s="7">
-        <v>6000000</v>
+        <v>10000000</v>
       </c>
       <c r="D82" s="8"/>
       <c r="E82" s="25"/>
     </row>
-    <row r="83" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:5" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A83" s="9">
         <v>99</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C83" s="7">
-        <f>SUM(C84:C92)</f>
-        <v>10000000</v>
+        <v>500000</v>
       </c>
       <c r="D83" s="8"/>
       <c r="E83" s="25"/>
     </row>
-    <row r="84" spans="1:5" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="9">
         <v>99</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C84" s="7">
         <v>500000</v>
@@ -3179,7 +3153,7 @@
         <v>99</v>
       </c>
       <c r="B85" s="6" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C85" s="7">
         <v>500000</v>
@@ -3192,7 +3166,7 @@
         <v>99</v>
       </c>
       <c r="B86" s="6" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C86" s="7">
         <v>500000</v>
@@ -3205,7 +3179,7 @@
         <v>99</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C87" s="7">
         <v>500000</v>
@@ -3218,7 +3192,7 @@
         <v>99</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C88" s="7">
         <v>500000</v>
@@ -3231,10 +3205,10 @@
         <v>99</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C89" s="7">
-        <v>500000</v>
+        <v>4000000</v>
       </c>
       <c r="D89" s="8"/>
       <c r="E89" s="25"/>
@@ -3244,10 +3218,10 @@
         <v>99</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C90" s="7">
-        <v>4000000</v>
+        <v>1000000</v>
       </c>
       <c r="D90" s="8"/>
       <c r="E90" s="25"/>
@@ -3257,10 +3231,10 @@
         <v>99</v>
       </c>
       <c r="B91" s="6" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C91" s="7">
-        <v>1000000</v>
+        <v>2000000</v>
       </c>
       <c r="D91" s="8"/>
       <c r="E91" s="25"/>
@@ -3270,10 +3244,10 @@
         <v>99</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C92" s="7">
-        <v>2000000</v>
+        <v>724523857</v>
       </c>
       <c r="D92" s="8"/>
       <c r="E92" s="25"/>
@@ -3283,11 +3257,10 @@
         <v>99</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C93" s="7">
-        <f>SUM(C94:C96)</f>
-        <v>724523857</v>
+        <v>217385530</v>
       </c>
       <c r="D93" s="8"/>
       <c r="E93" s="25"/>
@@ -3297,10 +3270,10 @@
         <v>99</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C94" s="7">
-        <v>217385530</v>
+        <v>40000000</v>
       </c>
       <c r="D94" s="8"/>
       <c r="E94" s="25"/>
@@ -3310,10 +3283,10 @@
         <v>99</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C95" s="7">
-        <v>40000000</v>
+        <v>467138327</v>
       </c>
       <c r="D95" s="8"/>
       <c r="E95" s="25"/>
@@ -3323,10 +3296,10 @@
         <v>99</v>
       </c>
       <c r="B96" s="6" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C96" s="7">
-        <v>467138327</v>
+        <v>111800000</v>
       </c>
       <c r="D96" s="8"/>
       <c r="E96" s="25"/>
@@ -3336,11 +3309,10 @@
         <v>99</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C97" s="7">
-        <f>SUM(C98:C99)</f>
-        <v>111800000</v>
+        <v>110000000</v>
       </c>
       <c r="D97" s="8"/>
       <c r="E97" s="25"/>
@@ -3350,10 +3322,10 @@
         <v>99</v>
       </c>
       <c r="B98" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C98" s="7">
-        <v>110000000</v>
+        <v>1800000</v>
       </c>
       <c r="D98" s="8"/>
       <c r="E98" s="25"/>
@@ -3363,12 +3335,12 @@
         <v>99</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C99" s="7">
-        <v>1800000</v>
-      </c>
-      <c r="D99" s="8"/>
+        <v>547120000</v>
+      </c>
+      <c r="D99" s="24"/>
       <c r="E99" s="25"/>
     </row>
     <row r="100" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3376,12 +3348,12 @@
         <v>99</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C100" s="7">
-        <v>547120000</v>
-      </c>
-      <c r="D100" s="24"/>
+        <v>100000000</v>
+      </c>
+      <c r="D100" s="8"/>
       <c r="E100" s="25"/>
     </row>
     <row r="101" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
@@ -3389,37 +3361,35 @@
         <v>99</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C101" s="7">
-        <v>100000000</v>
-      </c>
-      <c r="D101" s="8"/>
+        <v>447120000</v>
+      </c>
+      <c r="D101" s="24"/>
       <c r="E101" s="25"/>
     </row>
-    <row r="102" spans="1:5" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="9">
         <v>99</v>
       </c>
-      <c r="B102" s="6" t="s">
-        <v>133</v>
-      </c>
-      <c r="C102" s="7">
-        <v>447120000</v>
-      </c>
-      <c r="D102" s="24"/>
-      <c r="E102" s="25"/>
+      <c r="B102" t="s">
+        <v>131</v>
+      </c>
+      <c r="C102" s="2">
+        <v>599053289</v>
+      </c>
+      <c r="D102" s="25"/>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="9">
         <v>99</v>
       </c>
-      <c r="B103" t="s">
-        <v>134</v>
+      <c r="B103" s="6" t="s">
+        <v>132</v>
       </c>
       <c r="C103" s="2">
-        <f>C104+C113+C114+C120+C121+C122+C123+C124</f>
-        <v>599053289</v>
+        <v>332239129</v>
       </c>
       <c r="D103" s="25"/>
     </row>
@@ -3428,10 +3398,10 @@
         <v>99</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="C104" s="2">
-        <v>332239129</v>
+        <v>500000</v>
       </c>
       <c r="D104" s="25"/>
     </row>
@@ -3440,10 +3410,10 @@
         <v>99</v>
       </c>
       <c r="B105" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C105" s="2">
-        <v>500000</v>
+        <v>2000000</v>
       </c>
       <c r="D105" s="25"/>
     </row>
@@ -3452,34 +3422,34 @@
         <v>99</v>
       </c>
       <c r="B106" s="6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="C106" s="2">
-        <v>2000000</v>
-      </c>
-      <c r="D106" s="25"/>
+        <v>57486220</v>
+      </c>
+      <c r="D106" s="6"/>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="9">
         <v>99</v>
       </c>
       <c r="B107" s="6" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C107" s="2">
-        <v>57486220</v>
-      </c>
-      <c r="D107" s="6"/>
+        <v>250000000</v>
+      </c>
+      <c r="D107" s="25"/>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="9">
         <v>99</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="C108" s="2">
-        <v>250000000</v>
+        <v>16196279</v>
       </c>
       <c r="D108" s="25"/>
     </row>
@@ -3488,10 +3458,10 @@
         <v>99</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C109" s="2">
-        <v>16196279</v>
+        <v>85000000</v>
       </c>
       <c r="D109" s="25"/>
     </row>
@@ -3500,10 +3470,10 @@
         <v>99</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="C110" s="2">
-        <v>85000000</v>
+        <v>4684000</v>
       </c>
       <c r="D110" s="25"/>
     </row>
@@ -3512,10 +3482,10 @@
         <v>99</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C111" s="2">
-        <v>4684000</v>
+        <v>1287630</v>
       </c>
       <c r="D111" s="25"/>
     </row>
@@ -3524,22 +3494,21 @@
         <v>99</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C112" s="2">
-        <v>1287630</v>
-      </c>
-      <c r="D112" s="25"/>
+        <v>81280000</v>
+      </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="9">
         <v>99</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C113" s="2">
-        <v>81280000</v>
+        <v>19030950</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.25">
@@ -3547,11 +3516,10 @@
         <v>99</v>
       </c>
       <c r="B114" s="6" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C114" s="2">
-        <f>SUM(C115:C119)</f>
-        <v>19030950</v>
+        <v>1231900</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.25">
@@ -3559,10 +3527,10 @@
         <v>99</v>
       </c>
       <c r="B115" s="6" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C115" s="2">
-        <v>1231900</v>
+        <v>10814050</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.25">
@@ -3570,10 +3538,10 @@
         <v>99</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C116" s="2">
-        <v>10814050</v>
+        <v>3619500</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.25">
@@ -3581,10 +3549,10 @@
         <v>99</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C117" s="2">
-        <v>3619500</v>
+        <v>1651000</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.25">
@@ -3592,10 +3560,10 @@
         <v>99</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C118" s="2">
-        <v>1651000</v>
+        <v>1714500</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.25">
@@ -3603,33 +3571,33 @@
         <v>99</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C119" s="2">
-        <v>1714500</v>
-      </c>
+        <v>151050000</v>
+      </c>
+      <c r="D119" s="6"/>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="9">
         <v>99</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C120" s="2">
-        <v>151050000</v>
-      </c>
-      <c r="D120" s="6"/>
+        <v>939800</v>
+      </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="9">
         <v>99</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C121" s="2">
-        <v>939800</v>
+        <v>2933060</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.25">
@@ -3637,10 +3605,10 @@
         <v>99</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C122" s="2">
-        <v>2933060</v>
+        <v>4379450</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.25">
@@ -3648,46 +3616,44 @@
         <v>99</v>
       </c>
       <c r="B123" s="6" t="s">
+        <v>152</v>
+      </c>
+      <c r="C123" s="2">
+        <v>7200900</v>
+      </c>
+    </row>
+    <row r="124" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A124" s="9">
+        <v>99</v>
+      </c>
+      <c r="B124" s="6" t="s">
+        <v>153</v>
+      </c>
+      <c r="C124" s="5">
+        <v>2618708402</v>
+      </c>
+      <c r="E124" s="25"/>
+    </row>
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A125" s="9">
+        <v>99</v>
+      </c>
+      <c r="B125" s="6" t="s">
         <v>154</v>
       </c>
-      <c r="C123" s="2">
-        <v>4379450</v>
-      </c>
-    </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A124" s="9">
-        <v>99</v>
-      </c>
-      <c r="B124" s="6" t="s">
-        <v>155</v>
-      </c>
-      <c r="C124" s="2">
-        <v>7200900</v>
-      </c>
-    </row>
-    <row r="125" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A125" s="9">
-        <v>99</v>
-      </c>
-      <c r="B125" s="6" t="s">
-        <v>156</v>
-      </c>
-      <c r="C125" s="5">
-        <f>C126+C132+C135</f>
-        <v>2618708402</v>
-      </c>
-      <c r="E125" s="25"/>
+      <c r="C125" s="2">
+        <v>1003588402</v>
+      </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" s="9">
         <v>99</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C126" s="2">
-        <f>C127+C128+C129+C130+C131</f>
-        <v>1003588402</v>
+        <v>533000000</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.25">
@@ -3695,10 +3661,10 @@
         <v>99</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="C127" s="2">
-        <v>533000000</v>
+        <v>170000000</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.25">
@@ -3706,10 +3672,10 @@
         <v>99</v>
       </c>
       <c r="B128" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C128" s="2">
-        <v>170000000</v>
+        <v>45000000</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.25">
@@ -3717,10 +3683,10 @@
         <v>99</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C129" s="2">
-        <v>45000000</v>
+        <v>110000000</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.25">
@@ -3728,10 +3694,10 @@
         <v>99</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C130" s="2">
-        <v>110000000</v>
+        <v>145588402</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.25">
@@ -3739,10 +3705,10 @@
         <v>99</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C131" s="2">
-        <v>145588402</v>
+        <v>787400000</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.25">
@@ -3750,11 +3716,10 @@
         <v>99</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C132" s="2">
-        <f>C133+C134</f>
-        <v>787400000</v>
+        <v>620000000</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.25">
@@ -3762,10 +3727,10 @@
         <v>99</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C133" s="2">
-        <v>620000000</v>
+        <v>167400000</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.25">
@@ -3773,10 +3738,10 @@
         <v>99</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C134" s="2">
-        <v>167400000</v>
+        <v>827720000</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.25">
@@ -3784,11 +3749,10 @@
         <v>99</v>
       </c>
       <c r="B135" s="6" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C135" s="2">
-        <f>C136+C137+C138+C139+C140+C141+C142+C143</f>
-        <v>827720000</v>
+        <v>20000000</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.25">
@@ -3796,10 +3760,10 @@
         <v>99</v>
       </c>
       <c r="B136" s="6" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C136" s="2">
-        <v>20000000</v>
+        <v>69000000</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.25">
@@ -3807,10 +3771,10 @@
         <v>99</v>
       </c>
       <c r="B137" s="6" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C137" s="2">
-        <v>69000000</v>
+        <v>325000000</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.25">
@@ -3818,10 +3782,10 @@
         <v>99</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C138" s="2">
-        <v>325000000</v>
+        <v>173000000</v>
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.25">
@@ -3829,10 +3793,10 @@
         <v>99</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C139" s="2">
-        <v>173000000</v>
+        <v>15000000</v>
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.25">
@@ -3840,10 +3804,10 @@
         <v>99</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C140" s="2">
-        <v>15000000</v>
+        <v>24000000</v>
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.25">
@@ -3851,10 +3815,10 @@
         <v>99</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C141" s="2">
-        <v>24000000</v>
+        <v>30000000</v>
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.25">
@@ -3862,46 +3826,45 @@
         <v>99</v>
       </c>
       <c r="B142" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="C142" s="2">
+        <v>171720000</v>
+      </c>
+    </row>
+    <row r="143" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A143" s="9">
+        <v>99</v>
+      </c>
+      <c r="B143" s="6" t="s">
+        <v>172</v>
+      </c>
+      <c r="C143" s="5">
+        <v>1689100000</v>
+      </c>
+      <c r="E143" s="25"/>
+    </row>
+    <row r="144" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A144" s="9">
+        <v>99</v>
+      </c>
+      <c r="B144" s="6" t="s">
         <v>173</v>
       </c>
-      <c r="C142" s="2">
-        <v>30000000</v>
-      </c>
-    </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A143" s="9">
-        <v>99</v>
-      </c>
-      <c r="B143" s="6" t="s">
-        <v>174</v>
-      </c>
-      <c r="C143" s="2">
-        <v>171720000</v>
-      </c>
-    </row>
-    <row r="144" spans="1:5" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A144" s="9">
-        <v>99</v>
-      </c>
-      <c r="B144" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="C144" s="5">
-        <f>C145+C148+C156</f>
-        <v>1689100000</v>
-      </c>
-      <c r="E144" s="25"/>
+      <c r="C144" s="13">
+        <v>376000000</v>
+      </c>
+      <c r="E144" s="11"/>
     </row>
     <row r="145" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A145" s="9">
         <v>99</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="C145" s="13">
-        <f>C146+C147</f>
-        <v>376000000</v>
+        <v>174</v>
+      </c>
+      <c r="C145" s="14">
+        <v>356000000</v>
       </c>
       <c r="E145" s="11"/>
     </row>
@@ -3910,35 +3873,36 @@
         <v>99</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>177</v>
-      </c>
-      <c r="C146" s="14">
-        <v>356000000</v>
+        <v>175</v>
+      </c>
+      <c r="C146" s="13">
+        <v>20000000</v>
       </c>
       <c r="E146" s="11"/>
     </row>
-    <row r="147" spans="1:6" s="12" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A147" s="9">
         <v>99</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>178</v>
-      </c>
-      <c r="C147" s="13">
-        <v>20000000</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="C147" s="14">
+        <v>240000000</v>
+      </c>
+      <c r="D147" s="12"/>
       <c r="E147" s="11"/>
+      <c r="F147" s="12"/>
     </row>
     <row r="148" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A148" s="9">
         <v>99</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="C148" s="14">
-        <f>SUM(C149:C155)</f>
-        <v>240000000</v>
+        <v>177</v>
+      </c>
+      <c r="C148" s="16">
+        <v>500000</v>
       </c>
       <c r="D148" s="12"/>
       <c r="E148" s="11"/>
@@ -3949,10 +3913,10 @@
         <v>99</v>
       </c>
       <c r="B149" s="6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C149" s="16">
-        <v>500000</v>
+        <v>145000000</v>
       </c>
       <c r="D149" s="12"/>
       <c r="E149" s="11"/>
@@ -3963,10 +3927,10 @@
         <v>99</v>
       </c>
       <c r="B150" s="6" t="s">
-        <v>181</v>
-      </c>
-      <c r="C150" s="16">
-        <v>145000000</v>
+        <v>179</v>
+      </c>
+      <c r="C150" s="17">
+        <v>50000000</v>
       </c>
       <c r="D150" s="12"/>
       <c r="E150" s="11"/>
@@ -3977,10 +3941,10 @@
         <v>99</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="C151" s="17">
-        <v>50000000</v>
+        <v>180</v>
+      </c>
+      <c r="C151" s="16">
+        <v>7000000</v>
       </c>
       <c r="D151" s="12"/>
       <c r="E151" s="11"/>
@@ -3991,10 +3955,10 @@
         <v>99</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C152" s="16">
-        <v>7000000</v>
+        <v>4500000</v>
       </c>
       <c r="D152" s="12"/>
       <c r="E152" s="11"/>
@@ -4005,10 +3969,10 @@
         <v>99</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C153" s="16">
-        <v>4500000</v>
+        <v>17000000</v>
       </c>
       <c r="D153" s="12"/>
       <c r="E153" s="11"/>
@@ -4019,10 +3983,10 @@
         <v>99</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C154" s="16">
-        <v>17000000</v>
+        <v>16000000</v>
       </c>
       <c r="D154" s="12"/>
       <c r="E154" s="11"/>
@@ -4032,13 +3996,13 @@
       <c r="A155" s="9">
         <v>99</v>
       </c>
-      <c r="B155" s="6" t="s">
-        <v>186</v>
+      <c r="B155" s="18" t="s">
+        <v>184</v>
       </c>
       <c r="C155" s="16">
-        <v>16000000</v>
-      </c>
-      <c r="D155" s="12"/>
+        <v>1073100000</v>
+      </c>
+      <c r="D155" s="11"/>
       <c r="E155" s="11"/>
       <c r="F155" s="12"/>
     </row>
@@ -4046,51 +4010,36 @@
       <c r="A156" s="9">
         <v>99</v>
       </c>
-      <c r="B156" s="18" t="s">
-        <v>187</v>
-      </c>
-      <c r="C156" s="16">
-        <f>C157+C158</f>
-        <v>1073100000</v>
-      </c>
-      <c r="D156" s="11"/>
+      <c r="B156" s="15" t="s">
+        <v>185</v>
+      </c>
+      <c r="C156" s="14">
+        <v>400000000</v>
+      </c>
+      <c r="D156" s="12"/>
       <c r="E156" s="11"/>
       <c r="F156" s="12"/>
     </row>
-    <row r="157" spans="1:6" s="15" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A157" s="9">
         <v>99</v>
       </c>
-      <c r="B157" s="15" t="s">
-        <v>188</v>
-      </c>
-      <c r="C157" s="14">
-        <v>400000000</v>
-      </c>
-      <c r="D157" s="12"/>
-      <c r="E157" s="11"/>
-      <c r="F157" s="12"/>
+      <c r="B157" t="s">
+        <v>186</v>
+      </c>
+      <c r="C157" s="2">
+        <v>673100000</v>
+      </c>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A158" s="9">
-        <v>99</v>
-      </c>
-      <c r="B158" t="s">
-        <v>189</v>
-      </c>
-      <c r="C158" s="2">
-        <v>673100000</v>
-      </c>
+      <c r="A158" s="9"/>
+      <c r="D158" s="11"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A159" s="9"/>
-      <c r="D159" s="11"/>
+      <c r="A159"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A160"/>
-    </row>
-    <row r="161" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A161"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -4103,8 +4052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{629CCF99-671C-466C-8EB9-A95C45EF2C45}">
   <dimension ref="A1:C56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4115,7 +4064,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -4167,7 +4116,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="28" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="C6" s="28">
         <v>462309000</v>
@@ -4178,7 +4127,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="28" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C7" s="28">
         <v>5997600</v>
@@ -4189,7 +4138,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="28" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="C8" s="28">
         <v>11939410</v>
@@ -4200,7 +4149,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="28" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C9" s="28">
         <v>99559800</v>
@@ -4222,7 +4171,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="C11" s="2">
         <v>59121800</v>
@@ -4233,7 +4182,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="C12" s="2">
         <v>270785550</v>
@@ -4244,7 +4193,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="C13" s="2">
         <v>15282000</v>
@@ -4255,7 +4204,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C14" s="2">
         <v>811600</v>
@@ -4266,7 +4215,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="C15" s="2">
         <v>119679000</v>
@@ -4288,7 +4237,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C17" s="2">
         <v>100443284</v>
@@ -4299,7 +4248,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C18" s="2">
         <v>154589000</v>
@@ -4310,7 +4259,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="C19" s="2">
         <v>53810320</v>
@@ -4321,7 +4270,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="C20" s="2">
         <v>137494427</v>
@@ -4442,7 +4391,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="C31" s="2">
         <v>2285897273</v>
@@ -4519,7 +4468,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C38" s="2">
         <v>500000000</v>
@@ -4530,7 +4479,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="C39" s="2">
         <v>46700000</v>
@@ -4541,7 +4490,7 @@
         <v>99</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="C40" s="2">
         <v>65000000</v>
@@ -4596,7 +4545,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C45" s="2">
         <v>5000000</v>
@@ -4607,7 +4556,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="2" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="C46" s="2">
         <v>400000</v>
@@ -4618,7 +4567,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="2" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="C47" s="2">
         <v>1310255998</v>
@@ -4629,7 +4578,7 @@
         <v>99</v>
       </c>
       <c r="B48" s="2" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C48" s="2">
         <v>968100000</v>
@@ -4640,7 +4589,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="2" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="C49" s="2">
         <v>200000000</v>
@@ -4651,7 +4600,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="2" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="C50" s="2">
         <v>142155998</v>
@@ -4662,7 +4611,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="2" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="C51" s="2">
         <v>6712832403</v>
@@ -4673,7 +4622,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="2" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="C52" s="2">
         <v>1994660000</v>
@@ -4684,7 +4633,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="2" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="C53" s="2">
         <v>4718172403</v>
@@ -4695,7 +4644,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="2" t="s">
-        <v>208</v>
+        <v>380</v>
       </c>
       <c r="C54" s="2">
         <v>6712832403</v>
@@ -4767,7 +4716,7 @@
   <sheetData>
     <row r="1" spans="1:59" x14ac:dyDescent="0.25">
       <c r="A1" s="29" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
     </row>
     <row r="2" spans="1:59" x14ac:dyDescent="0.25">
@@ -4781,172 +4730,172 @@
         <v>1</v>
       </c>
       <c r="D2" s="29" t="s">
+        <v>309</v>
+      </c>
+      <c r="E2" s="29" t="s">
+        <v>310</v>
+      </c>
+      <c r="F2" s="29" t="s">
+        <v>311</v>
+      </c>
+      <c r="G2" s="29" t="s">
+        <v>312</v>
+      </c>
+      <c r="H2" s="29" t="s">
         <v>313</v>
       </c>
-      <c r="E2" s="29" t="s">
+      <c r="I2" s="29" t="s">
         <v>314</v>
       </c>
-      <c r="F2" s="29" t="s">
+      <c r="J2" s="29" t="s">
         <v>315</v>
       </c>
-      <c r="G2" s="29" t="s">
+      <c r="K2" s="29" t="s">
         <v>316</v>
       </c>
-      <c r="H2" s="29" t="s">
+      <c r="L2" s="29" t="s">
         <v>317</v>
       </c>
-      <c r="I2" s="29" t="s">
+      <c r="M2" s="29" t="s">
         <v>318</v>
       </c>
-      <c r="J2" s="29" t="s">
+      <c r="N2" s="29" t="s">
         <v>319</v>
       </c>
-      <c r="K2" s="29" t="s">
+      <c r="O2" s="29" t="s">
         <v>320</v>
       </c>
-      <c r="L2" s="29" t="s">
+      <c r="P2" s="29" t="s">
         <v>321</v>
       </c>
-      <c r="M2" s="29" t="s">
+      <c r="Q2" s="29" t="s">
         <v>322</v>
       </c>
-      <c r="N2" s="29" t="s">
+      <c r="R2" s="29" t="s">
         <v>323</v>
       </c>
-      <c r="O2" s="29" t="s">
+      <c r="S2" s="29" t="s">
         <v>324</v>
       </c>
-      <c r="P2" s="29" t="s">
+      <c r="T2" s="29" t="s">
         <v>325</v>
       </c>
-      <c r="Q2" s="29" t="s">
+      <c r="U2" s="29" t="s">
         <v>326</v>
       </c>
-      <c r="R2" s="29" t="s">
+      <c r="V2" s="29" t="s">
         <v>327</v>
       </c>
-      <c r="S2" s="29" t="s">
+      <c r="W2" s="29" t="s">
         <v>328</v>
       </c>
-      <c r="T2" s="29" t="s">
+      <c r="X2" s="29" t="s">
         <v>329</v>
       </c>
-      <c r="U2" s="29" t="s">
+      <c r="Y2" s="29" t="s">
         <v>330</v>
       </c>
-      <c r="V2" s="29" t="s">
+      <c r="Z2" s="29" t="s">
         <v>331</v>
       </c>
-      <c r="W2" s="29" t="s">
+      <c r="AA2" s="29" t="s">
         <v>332</v>
       </c>
-      <c r="X2" s="29" t="s">
+      <c r="AB2" s="29" t="s">
         <v>333</v>
       </c>
-      <c r="Y2" s="29" t="s">
+      <c r="AC2" s="29" t="s">
         <v>334</v>
       </c>
-      <c r="Z2" s="29" t="s">
+      <c r="AD2" s="29" t="s">
         <v>335</v>
       </c>
-      <c r="AA2" s="29" t="s">
+      <c r="AE2" s="29" t="s">
         <v>336</v>
       </c>
-      <c r="AB2" s="29" t="s">
+      <c r="AF2" s="29" t="s">
         <v>337</v>
       </c>
-      <c r="AC2" s="29" t="s">
+      <c r="AG2" s="29" t="s">
         <v>338</v>
       </c>
-      <c r="AD2" s="29" t="s">
+      <c r="AH2" s="29" t="s">
         <v>339</v>
       </c>
-      <c r="AE2" s="29" t="s">
+      <c r="AI2" s="29" t="s">
         <v>340</v>
       </c>
-      <c r="AF2" s="29" t="s">
+      <c r="AJ2" s="29" t="s">
         <v>341</v>
       </c>
-      <c r="AG2" s="29" t="s">
+      <c r="AK2" s="29" t="s">
         <v>342</v>
       </c>
-      <c r="AH2" s="29" t="s">
+      <c r="AL2" s="29" t="s">
         <v>343</v>
       </c>
-      <c r="AI2" s="29" t="s">
+      <c r="AM2" s="29" t="s">
         <v>344</v>
       </c>
-      <c r="AJ2" s="29" t="s">
+      <c r="AN2" s="29" t="s">
         <v>345</v>
       </c>
-      <c r="AK2" s="29" t="s">
+      <c r="AO2" s="29" t="s">
         <v>346</v>
       </c>
-      <c r="AL2" s="29" t="s">
+      <c r="AP2" s="29" t="s">
         <v>347</v>
       </c>
-      <c r="AM2" s="29" t="s">
+      <c r="AQ2" s="29" t="s">
         <v>348</v>
       </c>
-      <c r="AN2" s="29" t="s">
+      <c r="AR2" s="29" t="s">
         <v>349</v>
       </c>
-      <c r="AO2" s="29" t="s">
+      <c r="AS2" s="29" t="s">
         <v>350</v>
       </c>
-      <c r="AP2" s="29" t="s">
+      <c r="AT2" s="29" t="s">
         <v>351</v>
       </c>
-      <c r="AQ2" s="29" t="s">
+      <c r="AU2" s="29" t="s">
         <v>352</v>
       </c>
-      <c r="AR2" s="29" t="s">
+      <c r="AV2" s="29" t="s">
         <v>353</v>
       </c>
-      <c r="AS2" s="29" t="s">
+      <c r="AW2" s="29" t="s">
         <v>354</v>
       </c>
-      <c r="AT2" s="29" t="s">
+      <c r="AX2" s="29" t="s">
         <v>355</v>
       </c>
-      <c r="AU2" s="29" t="s">
+      <c r="AY2" s="29" t="s">
+        <v>313</v>
+      </c>
+      <c r="AZ2" s="29" t="s">
         <v>356</v>
       </c>
-      <c r="AV2" s="29" t="s">
+      <c r="BA2" s="29" t="s">
         <v>357</v>
       </c>
-      <c r="AW2" s="29" t="s">
+      <c r="BB2" s="29" t="s">
         <v>358</v>
       </c>
-      <c r="AX2" s="29" t="s">
+      <c r="BC2" s="29" t="s">
         <v>359</v>
       </c>
-      <c r="AY2" s="29" t="s">
-        <v>317</v>
-      </c>
-      <c r="AZ2" s="29" t="s">
+      <c r="BD2" s="29" t="s">
         <v>360</v>
       </c>
-      <c r="BA2" s="29" t="s">
+      <c r="BE2" s="29" t="s">
         <v>361</v>
       </c>
-      <c r="BB2" s="29" t="s">
+      <c r="BF2" s="29" t="s">
         <v>362</v>
       </c>
-      <c r="BC2" s="29" t="s">
-        <v>363</v>
-      </c>
-      <c r="BD2" s="29" t="s">
-        <v>364</v>
-      </c>
-      <c r="BE2" s="29" t="s">
-        <v>365</v>
-      </c>
-      <c r="BF2" s="29" t="s">
-        <v>366</v>
-      </c>
       <c r="BG2" s="29" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
     </row>
     <row r="3" spans="1:59" x14ac:dyDescent="0.25">
@@ -4954,7 +4903,7 @@
         <v>99</v>
       </c>
       <c r="B3" s="31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="32">
         <v>5103770263</v>
@@ -4965,7 +4914,7 @@
         <v>99</v>
       </c>
       <c r="B4" s="31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C4" s="32">
         <v>222768231</v>
@@ -4976,7 +4925,7 @@
         <v>99</v>
       </c>
       <c r="B5" s="31" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C5" s="32">
         <v>189960800</v>
@@ -4987,7 +4936,7 @@
         <v>99</v>
       </c>
       <c r="B6" s="31" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C6" s="32">
         <v>32807431</v>
@@ -4998,7 +4947,7 @@
         <v>99</v>
       </c>
       <c r="B7" s="31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C7" s="32">
         <v>2043364244</v>
@@ -5009,7 +4958,7 @@
         <v>99</v>
       </c>
       <c r="B8" s="31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="32">
         <v>1732037214</v>
@@ -5020,7 +4969,7 @@
         <v>99</v>
       </c>
       <c r="B9" s="31" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C9" s="32">
         <v>16842828</v>
@@ -5031,7 +4980,7 @@
         <v>99</v>
       </c>
       <c r="B10" s="31" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10" s="32">
         <v>294484202</v>
@@ -5042,7 +4991,7 @@
         <v>99</v>
       </c>
       <c r="B11" s="31" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11" s="32">
         <v>640438866</v>
@@ -5053,7 +5002,7 @@
         <v>99</v>
       </c>
       <c r="B12" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12" s="32">
         <v>93243562</v>
@@ -5064,7 +5013,7 @@
         <v>99</v>
       </c>
       <c r="B13" s="31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13" s="32">
         <v>79251341</v>
@@ -5075,7 +5024,7 @@
         <v>99</v>
       </c>
       <c r="B14" s="31" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14" s="32">
         <v>1000000</v>
@@ -5086,7 +5035,7 @@
         <v>99</v>
       </c>
       <c r="B15" s="31" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15" s="32">
         <v>12992221</v>
@@ -5097,7 +5046,7 @@
         <v>99</v>
       </c>
       <c r="B16" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16" s="32">
         <v>149693557</v>
@@ -5108,7 +5057,7 @@
         <v>99</v>
       </c>
       <c r="B17" s="31" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="32">
         <v>125277036</v>
@@ -5119,7 +5068,7 @@
         <v>99</v>
       </c>
       <c r="B18" s="31" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="32">
         <v>1734915</v>
@@ -5130,7 +5079,7 @@
         <v>99</v>
       </c>
       <c r="B19" s="31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C19" s="32">
         <v>22681606</v>
@@ -5141,7 +5090,7 @@
         <v>99</v>
       </c>
       <c r="B20" s="31" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C20" s="32">
         <v>104072380</v>
@@ -5152,7 +5101,7 @@
         <v>99</v>
       </c>
       <c r="B21" s="31" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C21" s="32">
         <v>89039212</v>
@@ -5163,7 +5112,7 @@
         <v>99</v>
       </c>
       <c r="B22" s="31" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C22" s="32">
         <v>578000</v>
@@ -5174,7 +5123,7 @@
         <v>99</v>
       </c>
       <c r="B23" s="31" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C23" s="32">
         <v>14455168</v>
@@ -5185,7 +5134,7 @@
         <v>99</v>
       </c>
       <c r="B24" s="31" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C24" s="32">
         <v>149086199</v>
@@ -5196,7 +5145,7 @@
         <v>99</v>
       </c>
       <c r="B25" s="31" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C25" s="32">
         <v>124929241</v>
@@ -5207,7 +5156,7 @@
         <v>99</v>
       </c>
       <c r="B26" s="31" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C26" s="32">
         <v>1370000</v>
@@ -5218,7 +5167,7 @@
         <v>99</v>
       </c>
       <c r="B27" s="31" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="32">
         <v>22786958</v>
@@ -5229,7 +5178,7 @@
         <v>99</v>
       </c>
       <c r="B28" s="31" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="32">
         <v>144343168</v>
@@ -5240,7 +5189,7 @@
         <v>99</v>
       </c>
       <c r="B29" s="31" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="32">
         <v>121478024</v>
@@ -5251,7 +5200,7 @@
         <v>99</v>
       </c>
       <c r="B30" s="31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="32">
         <v>1441000</v>
@@ -5262,7 +5211,7 @@
         <v>99</v>
       </c>
       <c r="B31" s="31" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="32">
         <v>21424144</v>
@@ -5273,7 +5222,7 @@
         <v>99</v>
       </c>
       <c r="B32" s="31" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="32">
         <v>1326100000</v>
@@ -5284,7 +5233,7 @@
         <v>99</v>
       </c>
       <c r="B33" s="31" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="32">
         <v>1120587200</v>
@@ -5295,7 +5244,7 @@
         <v>99</v>
       </c>
       <c r="B34" s="31" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C34" s="32">
         <v>17088000</v>
@@ -5306,7 +5255,7 @@
         <v>99</v>
       </c>
       <c r="B35" s="31" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C35" s="32">
         <v>188424800</v>
@@ -5317,7 +5266,7 @@
         <v>99</v>
       </c>
       <c r="B36" s="31" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C36" s="32">
         <v>42027890</v>
@@ -5328,7 +5277,7 @@
         <v>99</v>
       </c>
       <c r="B37" s="31" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C37" s="32">
         <v>34811556</v>
@@ -5339,7 +5288,7 @@
         <v>99</v>
       </c>
       <c r="B38" s="31" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C38" s="32">
         <v>1310000</v>
@@ -5350,7 +5299,7 @@
         <v>99</v>
       </c>
       <c r="B39" s="31" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C39" s="32">
         <v>5906334</v>
@@ -5361,7 +5310,7 @@
         <v>99</v>
       </c>
       <c r="B40" s="31" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="32">
         <v>300466210</v>
@@ -5372,7 +5321,7 @@
         <v>99</v>
       </c>
       <c r="B41" s="31" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C41" s="32">
         <v>247951691</v>
@@ -5383,7 +5332,7 @@
         <v>99</v>
       </c>
       <c r="B42" s="31" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C42" s="32">
         <v>6335400</v>
@@ -5394,7 +5343,7 @@
         <v>99</v>
       </c>
       <c r="B43" s="31" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C43" s="32">
         <v>46179119</v>
@@ -5405,7 +5354,7 @@
         <v>99</v>
       </c>
       <c r="B44" s="31" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C44" s="32">
         <v>223227098</v>
@@ -5416,7 +5365,7 @@
         <v>99</v>
       </c>
       <c r="B45" s="31" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" s="32">
         <v>188228592</v>
@@ -5427,7 +5376,7 @@
         <v>99</v>
       </c>
       <c r="B46" s="31" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C46" s="32">
         <v>1250000</v>
@@ -5438,7 +5387,7 @@
         <v>99</v>
       </c>
       <c r="B47" s="31" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C47" s="32">
         <v>33748506</v>
@@ -5449,7 +5398,7 @@
         <v>99</v>
       </c>
       <c r="B48" s="31" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C48" s="32">
         <v>305377724</v>
@@ -5460,7 +5409,7 @@
         <v>99</v>
       </c>
       <c r="B49" s="31" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C49" s="32">
         <v>259300317</v>
@@ -5471,7 +5420,7 @@
         <v>99</v>
       </c>
       <c r="B50" s="31" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C50" s="32">
         <v>250000</v>
@@ -5482,7 +5431,7 @@
         <v>99</v>
       </c>
       <c r="B51" s="31" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C51" s="32">
         <v>45827407</v>
@@ -5493,7 +5442,7 @@
         <v>99</v>
       </c>
       <c r="B52" s="31" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C52" s="32">
         <v>5554643775</v>
@@ -5504,7 +5453,7 @@
         <v>99</v>
       </c>
       <c r="B53" s="31" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C53" s="32">
         <v>4603346824</v>
@@ -5515,7 +5464,7 @@
         <v>99</v>
       </c>
       <c r="B54" s="31" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C54" s="33">
         <v>40477590</v>
@@ -5526,7 +5475,7 @@
         <v>99</v>
       </c>
       <c r="B55" s="31" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C55" s="33">
         <v>62775000</v>
@@ -5537,7 +5486,7 @@
         <v>99</v>
       </c>
       <c r="B56" s="31" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C56" s="33">
         <v>3171066602</v>
@@ -5548,7 +5497,7 @@
         <v>99</v>
       </c>
       <c r="B57" s="31" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="C57" s="33">
         <v>64100000</v>
@@ -5559,7 +5508,7 @@
         <v>99</v>
       </c>
       <c r="B58" s="31" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C58" s="33">
         <v>1264927632</v>
@@ -5570,7 +5519,7 @@
         <v>99</v>
       </c>
       <c r="B59" s="31" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="C59" s="32">
         <v>365086335</v>
@@ -5581,7 +5530,7 @@
         <v>99</v>
       </c>
       <c r="B60" s="31" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="C60" s="32">
         <v>36000000</v>
@@ -5592,7 +5541,7 @@
         <v>99</v>
       </c>
       <c r="B61" s="31" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C61" s="32">
         <v>47360000</v>
@@ -5603,7 +5552,7 @@
         <v>99</v>
       </c>
       <c r="B62" s="31" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="C62" s="32">
         <v>195455450</v>
@@ -5614,7 +5563,7 @@
         <v>99</v>
       </c>
       <c r="B63" s="31" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="C63" s="32">
         <v>0</v>
@@ -5625,7 +5574,7 @@
         <v>99</v>
       </c>
       <c r="B64" s="31" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="C64" s="32">
         <v>86270885</v>
@@ -5636,7 +5585,7 @@
         <v>99</v>
       </c>
       <c r="B65" s="31" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="C65" s="32">
         <v>78107500</v>
@@ -5647,7 +5596,7 @@
         <v>99</v>
       </c>
       <c r="B66" s="31" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C66" s="32">
         <v>10205750</v>
@@ -5658,7 +5607,7 @@
         <v>99</v>
       </c>
       <c r="B67" s="31" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C67" s="32">
         <v>18945750</v>
@@ -5669,7 +5618,7 @@
         <v>99</v>
       </c>
       <c r="B68" s="31" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C68" s="32">
         <v>14116750</v>
@@ -5680,7 +5629,7 @@
         <v>99</v>
       </c>
       <c r="B69" s="31" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C69" s="32">
         <v>15148150</v>
@@ -5691,7 +5640,7 @@
         <v>99</v>
       </c>
       <c r="B70" s="31" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C70" s="32">
         <v>19691100</v>
@@ -5702,7 +5651,7 @@
         <v>99</v>
       </c>
       <c r="B71" s="31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C71" s="32">
         <v>294000000</v>
@@ -5713,7 +5662,7 @@
         <v>99</v>
       </c>
       <c r="B72" s="31" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C72" s="32">
         <v>13207980</v>
@@ -5724,7 +5673,7 @@
         <v>99</v>
       </c>
       <c r="B73" s="31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C73" s="32">
         <v>103891480</v>
@@ -5735,7 +5684,7 @@
         <v>99</v>
       </c>
       <c r="B74" s="31" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C74" s="32">
         <v>40623646</v>
@@ -5746,7 +5695,7 @@
         <v>99</v>
       </c>
       <c r="B75" s="31" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C75" s="32">
         <v>56380010</v>
@@ -5757,7 +5706,7 @@
         <v>99</v>
       </c>
       <c r="B76" s="31" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C76" s="32">
         <v>408568000</v>
@@ -5768,7 +5717,7 @@
         <v>99</v>
       </c>
       <c r="B77" s="31" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C77" s="32">
         <v>126544000</v>
@@ -5779,7 +5728,7 @@
         <v>99</v>
       </c>
       <c r="B78" s="31" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
       <c r="C78" s="32">
         <v>35000000</v>
@@ -5790,7 +5739,7 @@
         <v>99</v>
       </c>
       <c r="B79" s="31" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C79" s="32">
         <v>7824000</v>
@@ -5801,7 +5750,7 @@
         <v>99</v>
       </c>
       <c r="B80" s="31" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="C80" s="32">
         <v>40000000</v>
@@ -5812,7 +5761,7 @@
         <v>99</v>
       </c>
       <c r="B81" s="31" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="C81" s="32">
         <v>1000000</v>
@@ -5823,7 +5772,7 @@
         <v>99</v>
       </c>
       <c r="B82" s="31" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="C82" s="32">
         <v>720000</v>
@@ -5834,7 +5783,7 @@
         <v>99</v>
       </c>
       <c r="B83" s="31" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="C83" s="32">
         <v>40000000</v>
@@ -5845,7 +5794,7 @@
         <v>99</v>
       </c>
       <c r="B84" s="31" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="C84" s="32">
         <v>2000000</v>
@@ -5856,7 +5805,7 @@
         <v>99</v>
       </c>
       <c r="B85" s="31" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="C85" s="32">
         <v>282024000</v>
@@ -5867,7 +5816,7 @@
         <v>99</v>
       </c>
       <c r="B86" s="31" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="C86" s="32">
         <v>50000000</v>
@@ -5878,7 +5827,7 @@
         <v>99</v>
       </c>
       <c r="B87" s="31" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="C87" s="32">
         <v>2000000</v>
@@ -5889,7 +5838,7 @@
         <v>99</v>
       </c>
       <c r="B88" s="31" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="C88" s="32">
         <v>12000000</v>
@@ -5900,7 +5849,7 @@
         <v>99</v>
       </c>
       <c r="B89" s="31" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C89" s="32">
         <v>3000000</v>
@@ -5911,7 +5860,7 @@
         <v>99</v>
       </c>
       <c r="B90" s="31" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C90" s="32">
         <v>80000000</v>
@@ -5922,7 +5871,7 @@
         <v>99</v>
       </c>
       <c r="B91" s="31" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="C91" s="32">
         <v>22500000</v>
@@ -5933,7 +5882,7 @@
         <v>99</v>
       </c>
       <c r="B92" s="31" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="C92" s="32">
         <v>8000000</v>
@@ -5944,7 +5893,7 @@
         <v>99</v>
       </c>
       <c r="B93" s="31" t="s">
-        <v>231</v>
+        <v>227</v>
       </c>
       <c r="C93" s="32">
         <v>500000</v>
@@ -5955,7 +5904,7 @@
         <v>99</v>
       </c>
       <c r="B94" s="31" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="C94" s="32">
         <v>22500000</v>
@@ -5966,7 +5915,7 @@
         <v>99</v>
       </c>
       <c r="B95" s="31" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="C95" s="32">
         <v>4250000</v>
@@ -5977,7 +5926,7 @@
         <v>99</v>
       </c>
       <c r="B96" s="31" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="C96" s="32">
         <v>1000000</v>
@@ -5988,7 +5937,7 @@
         <v>99</v>
       </c>
       <c r="B97" s="31" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="C97" s="32">
         <v>10000000</v>
@@ -5999,7 +5948,7 @@
         <v>99</v>
       </c>
       <c r="B98" s="31" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="C98" s="32">
         <v>66274000</v>
@@ -6010,7 +5959,7 @@
         <v>99</v>
       </c>
       <c r="B99" s="31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C99" s="32">
         <v>2706803035</v>
@@ -6021,7 +5970,7 @@
         <v>99</v>
       </c>
       <c r="B100" s="31" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="C100" s="32">
         <v>743201757</v>
@@ -6032,7 +5981,7 @@
         <v>99</v>
       </c>
       <c r="B101" s="31" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="C101" s="32">
         <v>41800000</v>
@@ -6043,7 +5992,7 @@
         <v>99</v>
       </c>
       <c r="B102" s="31" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="C102" s="32">
         <v>40000000</v>
@@ -6054,7 +6003,7 @@
         <v>99</v>
       </c>
       <c r="B103" s="31" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="C103" s="32">
         <v>1800000</v>
@@ -6065,7 +6014,7 @@
         <v>99</v>
       </c>
       <c r="B104" s="31" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="C104" s="32">
         <v>874501278</v>
@@ -6076,7 +6025,7 @@
         <v>99</v>
       </c>
       <c r="B105" s="31" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="C105" s="32">
         <v>40000000</v>
@@ -6087,7 +6036,7 @@
         <v>99</v>
       </c>
       <c r="B106" s="31" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="C106" s="32">
         <v>67100000</v>
@@ -6098,7 +6047,7 @@
         <v>99</v>
       </c>
       <c r="B107" s="31" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="C107" s="32">
         <v>17000000</v>
@@ -6109,7 +6058,7 @@
         <v>99</v>
       </c>
       <c r="B108" s="31" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="C108" s="32">
         <v>2400000</v>
@@ -6120,7 +6069,7 @@
         <v>99</v>
       </c>
       <c r="B109" s="31" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="C109" s="32">
         <v>32000000</v>
@@ -6131,7 +6080,7 @@
         <v>99</v>
       </c>
       <c r="B110" s="31" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C110" s="32">
         <v>2500000</v>
@@ -6142,7 +6091,7 @@
         <v>99</v>
       </c>
       <c r="B111" s="31" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C111" s="32">
         <v>6000000</v>
@@ -6153,7 +6102,7 @@
         <v>99</v>
       </c>
       <c r="B112" s="31" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C112" s="32">
         <v>2100000</v>
@@ -6164,7 +6113,7 @@
         <v>99</v>
       </c>
       <c r="B113" s="31" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C113" s="32">
         <v>3000000</v>
@@ -6175,7 +6124,7 @@
         <v>99</v>
       </c>
       <c r="B114" s="31" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C114" s="32">
         <v>100000</v>
@@ -6186,7 +6135,7 @@
         <v>99</v>
       </c>
       <c r="B115" s="31" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="C115" s="32">
         <v>2000000</v>
@@ -6197,7 +6146,7 @@
         <v>99</v>
       </c>
       <c r="B116" s="31" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="C116" s="32">
         <v>10500000</v>
@@ -6208,7 +6157,7 @@
         <v>99</v>
       </c>
       <c r="B117" s="31" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="C117" s="32">
         <v>500000</v>
@@ -6219,7 +6168,7 @@
         <v>99</v>
       </c>
       <c r="B118" s="31" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="C118" s="32">
         <v>500000</v>
@@ -6230,7 +6179,7 @@
         <v>99</v>
       </c>
       <c r="B119" s="31" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="C119" s="32">
         <v>500000</v>
@@ -6241,7 +6190,7 @@
         <v>99</v>
       </c>
       <c r="B120" s="31" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C120" s="32">
         <v>500000</v>
@@ -6252,7 +6201,7 @@
         <v>99</v>
       </c>
       <c r="B121" s="31" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="C121" s="32">
         <v>500000</v>
@@ -6263,7 +6212,7 @@
         <v>99</v>
       </c>
       <c r="B122" s="31" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="C122" s="32">
         <v>500000</v>
@@ -6274,7 +6223,7 @@
         <v>99</v>
       </c>
       <c r="B123" s="31" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="C123" s="32">
         <v>4000000</v>
@@ -6285,7 +6234,7 @@
         <v>99</v>
       </c>
       <c r="B124" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="C124" s="32">
         <v>1000000</v>
@@ -6296,7 +6245,7 @@
         <v>99</v>
       </c>
       <c r="B125" s="31" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="C125" s="32">
         <v>2000000</v>
@@ -6307,7 +6256,7 @@
         <v>99</v>
       </c>
       <c r="B126" s="31" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="C126" s="32">
         <v>500000</v>
@@ -6318,7 +6267,7 @@
         <v>99</v>
       </c>
       <c r="B127" s="31" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="C127" s="32">
         <v>17000000</v>
@@ -6329,7 +6278,7 @@
         <v>99</v>
       </c>
       <c r="B128" s="31" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="C128" s="32">
         <v>739901278</v>
@@ -6340,7 +6289,7 @@
         <v>99</v>
       </c>
       <c r="B129" s="31" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="C129" s="32">
         <v>211901278</v>
@@ -6351,7 +6300,7 @@
         <v>99</v>
       </c>
       <c r="B130" s="31" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C130" s="2">
         <v>528000000</v>
@@ -6362,7 +6311,7 @@
         <v>99</v>
       </c>
       <c r="B131" s="31" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="C131" s="32">
         <v>1047300000</v>
@@ -6373,7 +6322,7 @@
         <v>99</v>
       </c>
       <c r="B132" s="31" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C132" s="32">
         <v>100000000</v>
@@ -6384,7 +6333,7 @@
         <v>99</v>
       </c>
       <c r="B133" s="31" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="C133" s="32">
         <v>947300000</v>
@@ -6395,7 +6344,7 @@
         <v>99</v>
       </c>
       <c r="B134" s="31" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C134" s="2">
         <v>1301841058</v>
@@ -6406,7 +6355,7 @@
         <v>99</v>
       </c>
       <c r="B135" s="31" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C135" s="2">
         <v>1081323148</v>
@@ -6417,7 +6366,7 @@
         <v>99</v>
       </c>
       <c r="B136" s="31" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C136" s="2">
         <v>1287400</v>
@@ -6428,7 +6377,7 @@
         <v>99</v>
       </c>
       <c r="B137" s="31" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C137" s="2">
         <v>2000000</v>
@@ -6439,7 +6388,7 @@
         <v>99</v>
       </c>
       <c r="B138" s="31" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C138" s="2">
         <v>333345000</v>
@@ -6450,7 +6399,7 @@
         <v>99</v>
       </c>
       <c r="B139" s="31" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C139" s="2">
         <v>653800000</v>
@@ -6461,7 +6410,7 @@
         <v>99</v>
       </c>
       <c r="B140" s="31" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C140" s="2">
         <v>90890748</v>
@@ -6472,7 +6421,7 @@
         <v>99</v>
       </c>
       <c r="B141" s="31" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="C141" s="2">
         <v>5224780</v>
@@ -6483,7 +6432,7 @@
         <v>99</v>
       </c>
       <c r="B142" s="31" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="C142" s="32">
         <v>81280000</v>
@@ -6494,7 +6443,7 @@
         <v>99</v>
       </c>
       <c r="B143" s="31" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C143" s="32">
         <v>16192500</v>
@@ -6505,7 +6454,7 @@
         <v>99</v>
       </c>
       <c r="B144" s="31" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C144" s="32">
         <v>94791110</v>
@@ -6516,7 +6465,7 @@
         <v>99</v>
       </c>
       <c r="B145" s="31" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="C145" s="32">
         <v>811685</v>
@@ -6527,7 +6476,7 @@
         <v>99</v>
       </c>
       <c r="B146" s="31" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="C146" s="32">
         <v>2325388</v>
@@ -6538,7 +6487,7 @@
         <v>99</v>
       </c>
       <c r="B147" s="31" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="C147" s="32">
         <v>16946047</v>
@@ -6549,7 +6498,7 @@
         <v>99</v>
       </c>
       <c r="B148" s="31" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="C148" s="32">
         <v>2946400</v>
@@ -6560,7 +6509,7 @@
         <v>99</v>
       </c>
       <c r="B149" s="31" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="C149" s="2">
         <v>3585732832</v>
@@ -6571,7 +6520,7 @@
         <v>99</v>
       </c>
       <c r="B150" s="31" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C150" s="2">
         <v>330962000</v>
@@ -6582,7 +6531,7 @@
         <v>99</v>
       </c>
       <c r="B151" s="31" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C151" s="2">
         <v>65000000</v>
@@ -6593,7 +6542,7 @@
         <v>99</v>
       </c>
       <c r="B152" s="31" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C152" s="2">
         <v>100000000</v>
@@ -6604,7 +6553,7 @@
         <v>99</v>
       </c>
       <c r="B153" s="31" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C153" s="2">
         <v>25000000</v>
@@ -6615,7 +6564,7 @@
         <v>99</v>
       </c>
       <c r="B154" s="31" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C154" s="2">
         <v>70600000</v>
@@ -6626,7 +6575,7 @@
         <v>99</v>
       </c>
       <c r="B155" s="31" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C155" s="2">
         <v>70362000</v>
@@ -6637,7 +6586,7 @@
         <v>99</v>
       </c>
       <c r="B156" s="31" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="C156" s="2">
         <v>796290000</v>
@@ -6648,7 +6597,7 @@
         <v>99</v>
       </c>
       <c r="B157" s="31" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C157" s="2">
         <v>613000000</v>
@@ -6659,7 +6608,7 @@
         <v>99</v>
       </c>
       <c r="B158" s="31" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C158" s="2">
         <v>5000000</v>
@@ -6670,7 +6619,7 @@
         <v>99</v>
       </c>
       <c r="B159" s="31" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C159" s="2">
         <v>9000000</v>
@@ -6681,7 +6630,7 @@
         <v>99</v>
       </c>
       <c r="B160" s="31" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C160" s="2">
         <v>169290000</v>
@@ -6692,7 +6641,7 @@
         <v>99</v>
       </c>
       <c r="B161" s="31" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C161" s="2">
         <v>648063647</v>
@@ -6703,7 +6652,7 @@
         <v>99</v>
       </c>
       <c r="B162" s="31" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C162" s="2">
         <v>20000000</v>
@@ -6714,7 +6663,7 @@
         <v>99</v>
       </c>
       <c r="B163" s="31" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="C163" s="2">
         <v>20000000</v>
@@ -6725,7 +6674,7 @@
         <v>99</v>
       </c>
       <c r="B164" s="31" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="C164" s="2">
         <v>120000000</v>
@@ -6736,7 +6685,7 @@
         <v>99</v>
       </c>
       <c r="B165" s="31" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="C165" s="2">
         <v>60000000</v>
@@ -6747,7 +6696,7 @@
         <v>99</v>
       </c>
       <c r="B166" s="31" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="C166" s="2">
         <v>265000000</v>
@@ -6758,7 +6707,7 @@
         <v>99</v>
       </c>
       <c r="B167" s="31" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="C167" s="2">
         <v>110000000</v>
@@ -6769,7 +6718,7 @@
         <v>99</v>
       </c>
       <c r="B168" s="31" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C168" s="2">
         <v>19000000</v>
@@ -6780,7 +6729,7 @@
         <v>99</v>
       </c>
       <c r="B169" s="31" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="C169" s="2">
         <v>34063647</v>
@@ -6791,7 +6740,7 @@
         <v>99</v>
       </c>
       <c r="B170" s="31" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="C170" s="2">
         <v>1292000000</v>
@@ -6802,7 +6751,7 @@
         <v>99</v>
       </c>
       <c r="B171" s="31" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="C171" s="2">
         <v>510000000</v>
@@ -6813,7 +6762,7 @@
         <v>99</v>
       </c>
       <c r="B172" s="31" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="C172" s="2">
         <v>50000000</v>
@@ -6824,7 +6773,7 @@
         <v>99</v>
       </c>
       <c r="B173" s="31" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="C173" s="2">
         <v>6000000</v>
@@ -6835,7 +6784,7 @@
         <v>99</v>
       </c>
       <c r="B174" s="31" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="C174" s="2">
         <v>5000000</v>
@@ -6846,7 +6795,7 @@
         <v>99</v>
       </c>
       <c r="B175" s="31" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C175" s="2">
         <v>15000000</v>
@@ -6857,7 +6806,7 @@
         <v>99</v>
       </c>
       <c r="B176" s="31" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C176" s="2">
         <v>46000000</v>
@@ -6868,7 +6817,7 @@
         <v>99</v>
       </c>
       <c r="B177" s="31" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C177" s="2">
         <v>400000000</v>
@@ -6879,7 +6828,7 @@
         <v>99</v>
       </c>
       <c r="B178" s="31" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="C178" s="2">
         <v>5000000</v>
@@ -6890,7 +6839,7 @@
         <v>99</v>
       </c>
       <c r="B179" s="31" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="C179" s="2">
         <v>30000000</v>
@@ -6901,7 +6850,7 @@
         <v>99</v>
       </c>
       <c r="B180" s="31" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="C180" s="2">
         <v>50000000</v>
@@ -6912,7 +6861,7 @@
         <v>99</v>
       </c>
       <c r="B181" s="31" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="C181" s="2">
         <v>15000000</v>
@@ -6923,7 +6872,7 @@
         <v>99</v>
       </c>
       <c r="B182" s="31" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="C182" s="2">
         <v>160000000</v>
@@ -6934,7 +6883,7 @@
         <v>99</v>
       </c>
       <c r="B183" s="31" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="C183" s="2">
         <v>518417185</v>
@@ -6945,7 +6894,7 @@
         <v>99</v>
       </c>
       <c r="B184" s="31" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C184" s="2">
         <v>812243942</v>
@@ -6956,7 +6905,7 @@
         <v>99</v>
       </c>
       <c r="B185" s="31" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="C185" s="2">
         <v>355500000</v>
@@ -6967,7 +6916,7 @@
         <v>99</v>
       </c>
       <c r="B186" s="31" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="C186" s="2">
         <v>345500000</v>
@@ -6978,7 +6927,7 @@
         <v>99</v>
       </c>
       <c r="B187" s="31" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="C187" s="2">
         <v>10000000</v>
@@ -6989,7 +6938,7 @@
         <v>99</v>
       </c>
       <c r="B188" s="31" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C188" s="2">
         <v>226743942</v>
@@ -7000,7 +6949,7 @@
         <v>99</v>
       </c>
       <c r="B189" s="31" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="C189" s="34">
         <v>500000</v>
@@ -7011,7 +6960,7 @@
         <v>99</v>
       </c>
       <c r="B190" s="31" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C190" s="34">
         <v>145000000</v>
@@ -7022,7 +6971,7 @@
         <v>99</v>
       </c>
       <c r="B191" s="31" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="C191" s="35">
         <v>30000000</v>
@@ -7033,7 +6982,7 @@
         <v>99</v>
       </c>
       <c r="B192" s="31" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="C192" s="34">
         <v>5243942</v>
@@ -7044,7 +6993,7 @@
         <v>99</v>
       </c>
       <c r="B193" s="31" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C193" s="34">
         <v>15000000</v>
@@ -7055,7 +7004,7 @@
         <v>99</v>
       </c>
       <c r="B194" s="31" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C194" s="34">
         <v>10000000</v>
@@ -7066,7 +7015,7 @@
         <v>99</v>
       </c>
       <c r="B195" s="31" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C195" s="34">
         <v>5000000</v>
@@ -7077,7 +7026,7 @@
         <v>99</v>
       </c>
       <c r="B196" s="31" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C196" s="34">
         <v>5000000</v>
@@ -7088,7 +7037,7 @@
         <v>99</v>
       </c>
       <c r="B197" s="31" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C197" s="34">
         <v>3000000</v>
@@ -7099,7 +7048,7 @@
         <v>99</v>
       </c>
       <c r="B198" s="31" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C198" s="34">
         <v>8000000</v>
@@ -7110,7 +7059,7 @@
         <v>99</v>
       </c>
       <c r="B199" s="31" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C199" s="34">
         <v>30000000</v>
@@ -7121,7 +7070,7 @@
         <v>99</v>
       </c>
       <c r="B200" s="31" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C200" s="34">
         <v>30000000</v>
@@ -7132,7 +7081,7 @@
         <v>99</v>
       </c>
       <c r="B201" s="31" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="C201" s="34">
         <v>200000000</v>
@@ -7143,7 +7092,7 @@
         <v>99</v>
       </c>
       <c r="B202" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="C202" s="2">
         <v>19473602905</v>

</xml_diff>

<commit_message>
added new config, budget and milestone pics
</commit_message>
<xml_diff>
--- a/input/budget.xlsx
+++ b/input/budget.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4784027176d9b30c/_KMONITOR/_KÖKÖ/JÓZSEFVÁROS_KÖKÖ/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="15" documentId="8_{E6C61E6A-64E9-4903-9915-7A6217DEA31C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{8F9DF125-F397-4D74-927C-201704554485}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{E6C61E6A-64E9-4903-9915-7A6217DEA31C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{43946407-363D-4FB7-A67E-5F1F3D217528}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{A5FFBDF2-3FC8-479A-A77C-B32FE37E1D3D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{A5FFBDF2-3FC8-479A-A77C-B32FE37E1D3D}"/>
   </bookViews>
   <sheets>
     <sheet name="2021 BEVÉTEL" sheetId="1" r:id="rId1"/>
@@ -144,24 +144,6 @@
     <t>Tulajdonosi bevételek (B3101)</t>
   </si>
   <si>
-    <t>Parkolási bevétel (B310301)</t>
-  </si>
-  <si>
-    <t>Helyiségbérletidíj-bevétel (B310302)</t>
-  </si>
-  <si>
-    <t>Lakásbérletidíj-bevétel (B310303)</t>
-  </si>
-  <si>
-    <t>Telek és egyéb inatlanok  utáni bérleti díjbevétel  (B310304)</t>
-  </si>
-  <si>
-    <t>Piacüzemeltetésből származó bevétel (B310305)</t>
-  </si>
-  <si>
-    <t>Egyéb tulajdonnal összefüggő bevétel (víz, csatorna, szemét, fűtés) (B310306)</t>
-  </si>
-  <si>
     <t>Ellátási díjak (B3102)</t>
   </si>
   <si>
@@ -222,12 +204,6 @@
     <t>Felhalmozási célú átvett pénzeszközök államháztartáson kívülről (B43)</t>
   </si>
   <si>
-    <t>Munkáltatói kölcsön megtérülés (B3401)</t>
-  </si>
-  <si>
-    <t>Társasházak visszatérítendő kölcsönbevétele (B3402)</t>
-  </si>
-  <si>
     <t>Finanszírozási bevételek (B5)</t>
   </si>
   <si>
@@ -655,6 +631,30 @@
   </si>
   <si>
     <t>Finanszírozási kiadások (K8)</t>
+  </si>
+  <si>
+    <t>Parkolási bevétel (B310101)</t>
+  </si>
+  <si>
+    <t>Helyiségbérletidíj-bevétel (B310102)</t>
+  </si>
+  <si>
+    <t>Lakásbérletidíj-bevétel (B310103)</t>
+  </si>
+  <si>
+    <t>Piacüzemeltetésből származó bevétel (B310105)</t>
+  </si>
+  <si>
+    <t>Egyéb tulajdonnal összefüggő bevétel (víz, csatorna, szemét, fűtés) (B310106)</t>
+  </si>
+  <si>
+    <t>Telek és egyéb ingatlanok  utáni bérleti díjbevétel  (B310104)</t>
+  </si>
+  <si>
+    <t>Munkáltatói kölcsön megtérülés (B4301)</t>
+  </si>
+  <si>
+    <t>Társasházak visszatérítendő kölcsönbevétele (B4302)</t>
   </si>
 </sst>
 </file>
@@ -1026,8 +1026,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{13CA9AEA-E1B4-4D04-A721-BE3256AB9353}">
   <dimension ref="A1:C65"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B67" sqref="B67"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1398,7 +1398,7 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>199</v>
       </c>
       <c r="C34" s="4">
         <v>1172102079</v>
@@ -1409,7 +1409,7 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>37</v>
+        <v>200</v>
       </c>
       <c r="C35" s="4">
         <v>592913000</v>
@@ -1420,7 +1420,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>38</v>
+        <v>201</v>
       </c>
       <c r="C36" s="4">
         <v>686400000</v>
@@ -1431,7 +1431,7 @@
         <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>39</v>
+        <v>204</v>
       </c>
       <c r="C37" s="4">
         <v>80228181</v>
@@ -1442,7 +1442,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>202</v>
       </c>
       <c r="C38" s="4">
         <v>56722503</v>
@@ -1453,7 +1453,7 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>41</v>
+        <v>203</v>
       </c>
       <c r="C39" s="4">
         <v>284145598</v>
@@ -1464,7 +1464,7 @@
         <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="C40" s="4">
         <v>134038000</v>
@@ -1475,7 +1475,7 @@
         <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="C41" s="4">
         <v>690708894</v>
@@ -1486,7 +1486,7 @@
         <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="C42" s="4">
         <v>76081000</v>
@@ -1497,7 +1497,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C43" s="4">
         <v>172669000</v>
@@ -1508,7 +1508,7 @@
         <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="C44" s="4">
         <v>165733095</v>
@@ -1519,7 +1519,7 @@
         <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="C45" s="4">
         <v>245674158</v>
@@ -1530,7 +1530,7 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="C46" s="4">
         <v>14886000</v>
@@ -1541,7 +1541,7 @@
         <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C47" s="4">
         <v>134928814</v>
@@ -1552,7 +1552,7 @@
         <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C48" s="4">
         <v>95859344</v>
@@ -1563,7 +1563,7 @@
         <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C49" s="4">
         <v>2638243021</v>
@@ -1574,7 +1574,7 @@
         <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C50" s="4">
         <v>1992679007</v>
@@ -1585,7 +1585,7 @@
         <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C51" s="4">
         <v>428000000</v>
@@ -1596,7 +1596,7 @@
         <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="C52" s="4">
         <v>160000000</v>
@@ -1607,7 +1607,7 @@
         <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="C53" s="4">
         <v>253937007</v>
@@ -1618,7 +1618,7 @@
         <v>99</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="C54" s="4">
         <v>1150742000</v>
@@ -1629,7 +1629,7 @@
         <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C55" s="4">
         <v>395286014</v>
@@ -1640,7 +1640,7 @@
         <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C56" s="4">
         <v>39250000</v>
@@ -1651,7 +1651,7 @@
         <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="C57" s="4">
         <v>270000000</v>
@@ -1662,7 +1662,7 @@
         <v>99</v>
       </c>
       <c r="B58" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C58" s="4">
         <v>86036014</v>
@@ -1673,7 +1673,7 @@
         <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="C59" s="4">
         <v>250278000</v>
@@ -1684,7 +1684,7 @@
         <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>62</v>
+        <v>205</v>
       </c>
       <c r="C60" s="4">
         <v>278000</v>
@@ -1695,7 +1695,7 @@
         <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>63</v>
+        <v>206</v>
       </c>
       <c r="C61" s="4">
         <v>250000000</v>
@@ -1706,7 +1706,7 @@
         <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="C62" s="4">
         <v>8030774463</v>
@@ -1717,7 +1717,7 @@
         <v>99</v>
       </c>
       <c r="B63" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C63" s="4">
         <v>4117832424</v>
@@ -1728,7 +1728,7 @@
         <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C64" s="4">
         <v>3912942039</v>
@@ -1739,7 +1739,7 @@
         <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="C65" s="4">
         <v>7914544871</v>
@@ -1754,7 +1754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B44BE7C-5B22-4514-95C7-E57F7DD5CD66}">
   <dimension ref="A1:C202"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F144" sqref="F144"/>
     </sheetView>
   </sheetViews>
@@ -1786,7 +1786,7 @@
         <v>99</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C3" s="4">
         <v>7704289861</v>
@@ -1797,7 +1797,7 @@
         <v>99</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="C4" s="4">
         <v>277167630</v>
@@ -1808,7 +1808,7 @@
         <v>99</v>
       </c>
       <c r="B5" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C5" s="4">
         <v>1878168231</v>
@@ -1819,7 +1819,7 @@
         <v>99</v>
       </c>
       <c r="B6" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C6" s="4">
         <v>1157279000</v>
@@ -1830,7 +1830,7 @@
         <v>99</v>
       </c>
       <c r="B7" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C7" s="4">
         <v>893865000</v>
@@ -1841,7 +1841,7 @@
         <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C8" s="4">
         <v>2227121000</v>
@@ -1852,7 +1852,7 @@
         <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C9" s="4">
         <v>1270689000</v>
@@ -1863,7 +1863,7 @@
         <v>99</v>
       </c>
       <c r="B10" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C10" s="4">
         <v>7439824109</v>
@@ -1874,7 +1874,7 @@
         <v>99</v>
       </c>
       <c r="B11" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C11" s="4">
         <v>5363538343</v>
@@ -1885,7 +1885,7 @@
         <v>99</v>
       </c>
       <c r="B12" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4">
         <v>4353154945</v>
@@ -1896,7 +1896,7 @@
         <v>99</v>
       </c>
       <c r="B13" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C13" s="4">
         <v>801068498</v>
@@ -1907,7 +1907,7 @@
         <v>99</v>
       </c>
       <c r="B14" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="C14" s="4">
         <v>171022800</v>
@@ -1918,7 +1918,7 @@
         <v>99</v>
       </c>
       <c r="B15" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C15" s="4">
         <v>45765000</v>
@@ -1929,7 +1929,7 @@
         <v>99</v>
       </c>
       <c r="B16" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C16" s="4">
         <v>2921279930</v>
@@ -1940,7 +1940,7 @@
         <v>99</v>
       </c>
       <c r="B17" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C17" s="4">
         <v>414018717</v>
@@ -1951,7 +1951,7 @@
         <v>99</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="C18" s="4">
         <v>7290000</v>
@@ -1962,7 +1962,7 @@
         <v>99</v>
       </c>
       <c r="B19" t="s">
-        <v>84</v>
+        <v>76</v>
       </c>
       <c r="C19" s="4">
         <v>1003093398</v>
@@ -1973,7 +1973,7 @@
         <v>99</v>
       </c>
       <c r="B20" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="C20" s="4">
         <v>445083086</v>
@@ -1984,7 +1984,7 @@
         <v>99</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="C21" s="4">
         <v>927108680</v>
@@ -1995,7 +1995,7 @@
         <v>99</v>
       </c>
       <c r="B22" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="C22" s="4">
         <v>233671000</v>
@@ -2006,7 +2006,7 @@
         <v>99</v>
       </c>
       <c r="B23" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
       <c r="C23" s="4">
         <v>366866000</v>
@@ -2017,7 +2017,7 @@
         <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
       <c r="C24" s="4">
         <v>103557000</v>
@@ -2028,7 +2028,7 @@
         <v>99</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
       <c r="C25" s="4">
         <v>119429000</v>
@@ -2039,7 +2039,7 @@
         <v>99</v>
       </c>
       <c r="B26" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C26" s="4">
         <v>30000000</v>
@@ -2050,7 +2050,7 @@
         <v>99</v>
       </c>
       <c r="B27" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
       <c r="C27" s="4">
         <v>3200000</v>
@@ -2061,7 +2061,7 @@
         <v>99</v>
       </c>
       <c r="B28" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
       <c r="C28" s="4">
         <v>9000000</v>
@@ -2072,7 +2072,7 @@
         <v>99</v>
       </c>
       <c r="B29" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
       <c r="C29" s="4">
         <v>18000000</v>
@@ -2083,7 +2083,7 @@
         <v>99</v>
       </c>
       <c r="B30" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
       <c r="C30" s="4">
         <v>2500000</v>
@@ -2094,7 +2094,7 @@
         <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C31" s="4">
         <v>6000000</v>
@@ -2105,7 +2105,7 @@
         <v>99</v>
       </c>
       <c r="B32" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
       <c r="C32" s="4">
         <v>25000000</v>
@@ -2116,7 +2116,7 @@
         <v>99</v>
       </c>
       <c r="B33" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
       <c r="C33" s="4">
         <v>3000000</v>
@@ -2127,7 +2127,7 @@
         <v>99</v>
       </c>
       <c r="B34" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="C34" s="4">
         <v>3000000</v>
@@ -2138,7 +2138,7 @@
         <v>99</v>
       </c>
       <c r="B35" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
       <c r="C35" s="4">
         <v>4000000</v>
@@ -2149,7 +2149,7 @@
         <v>99</v>
       </c>
       <c r="B36" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C36" s="4">
         <v>4500000</v>
@@ -2160,7 +2160,7 @@
         <v>99</v>
       </c>
       <c r="B37" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C37" s="4">
         <v>10000000</v>
@@ -2171,7 +2171,7 @@
         <v>99</v>
       </c>
       <c r="B38" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
       <c r="C38" s="4">
         <v>1229000</v>
@@ -2182,7 +2182,7 @@
         <v>99</v>
       </c>
       <c r="B39" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C39" s="4">
         <v>4374934878</v>
@@ -2193,7 +2193,7 @@
         <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C40" s="4">
         <v>990715951</v>
@@ -2204,7 +2204,7 @@
         <v>99</v>
       </c>
       <c r="B41" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C41" s="4">
         <v>37000000</v>
@@ -2215,7 +2215,7 @@
         <v>99</v>
       </c>
       <c r="B42" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C42" s="4">
         <v>946890950</v>
@@ -2226,7 +2226,7 @@
         <v>99</v>
       </c>
       <c r="B43" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C43" s="4">
         <v>6825001</v>
@@ -2237,7 +2237,7 @@
         <v>99</v>
       </c>
       <c r="B44" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="C44" s="4">
         <v>126150000</v>
@@ -2248,7 +2248,7 @@
         <v>99</v>
       </c>
       <c r="B45" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
       <c r="C45" s="4">
         <v>2650000</v>
@@ -2259,7 +2259,7 @@
         <v>99</v>
       </c>
       <c r="B46" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C46" s="4">
         <v>50000000</v>
@@ -2270,7 +2270,7 @@
         <v>99</v>
       </c>
       <c r="B47" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="C47" s="4">
         <v>65000000</v>
@@ -2281,7 +2281,7 @@
         <v>99</v>
       </c>
       <c r="B48" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C48" s="4">
         <v>8500000</v>
@@ -2292,7 +2292,7 @@
         <v>99</v>
       </c>
       <c r="B49" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
       <c r="C49" s="4">
         <v>2117072473</v>
@@ -2303,7 +2303,7 @@
         <v>99</v>
       </c>
       <c r="B50" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C50" s="4">
         <v>6514000</v>
@@ -2314,7 +2314,7 @@
         <v>99</v>
       </c>
       <c r="B51" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
       <c r="C51" s="4">
         <v>1000000</v>
@@ -2325,7 +2325,7 @@
         <v>99</v>
       </c>
       <c r="B52" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C52" s="4">
         <v>3896000</v>
@@ -2336,7 +2336,7 @@
         <v>99</v>
       </c>
       <c r="B53" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="C53" s="4">
         <v>37743688</v>
@@ -2347,7 +2347,7 @@
         <v>99</v>
       </c>
       <c r="B54" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C54" s="4">
         <v>1346110300</v>
@@ -2358,7 +2358,7 @@
         <v>99</v>
       </c>
       <c r="B55" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C55" s="4">
         <v>122142564</v>
@@ -2369,7 +2369,7 @@
         <v>99</v>
       </c>
       <c r="B56" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C56" s="4">
         <v>599665921</v>
@@ -2380,7 +2380,7 @@
         <v>99</v>
       </c>
       <c r="B57" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
       <c r="C57" s="4">
         <v>200000000</v>
@@ -2391,7 +2391,7 @@
         <v>99</v>
       </c>
       <c r="B58" t="s">
-        <v>123</v>
+        <v>115</v>
       </c>
       <c r="C58" s="4">
         <v>940996454</v>
@@ -2402,7 +2402,7 @@
         <v>99</v>
       </c>
       <c r="B59" t="s">
-        <v>124</v>
+        <v>116</v>
       </c>
       <c r="C59" s="4">
         <v>4239768354</v>
@@ -2413,7 +2413,7 @@
         <v>99</v>
       </c>
       <c r="B60" t="s">
-        <v>125</v>
+        <v>117</v>
       </c>
       <c r="C60" s="4">
         <v>138127905</v>
@@ -2424,7 +2424,7 @@
         <v>99</v>
       </c>
       <c r="B61" t="s">
-        <v>126</v>
+        <v>118</v>
       </c>
       <c r="C61" s="4">
         <v>61511285</v>
@@ -2435,7 +2435,7 @@
         <v>99</v>
       </c>
       <c r="B62" t="s">
-        <v>127</v>
+        <v>119</v>
       </c>
       <c r="C62" s="4">
         <v>54998620</v>
@@ -2446,7 +2446,7 @@
         <v>99</v>
       </c>
       <c r="B63" t="s">
-        <v>128</v>
+        <v>120</v>
       </c>
       <c r="C63" s="4">
         <v>10618000</v>
@@ -2457,7 +2457,7 @@
         <v>99</v>
       </c>
       <c r="B64" t="s">
-        <v>129</v>
+        <v>121</v>
       </c>
       <c r="C64" s="4">
         <v>4000000</v>
@@ -2468,7 +2468,7 @@
         <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="C65" s="4">
         <v>7000000</v>
@@ -2479,7 +2479,7 @@
         <v>99</v>
       </c>
       <c r="B66" t="s">
-        <v>131</v>
+        <v>123</v>
       </c>
       <c r="C66" s="4">
         <v>992233000</v>
@@ -2490,7 +2490,7 @@
         <v>99</v>
       </c>
       <c r="B67" t="s">
-        <v>132</v>
+        <v>124</v>
       </c>
       <c r="C67" s="4">
         <v>618482000</v>
@@ -2501,7 +2501,7 @@
         <v>99</v>
       </c>
       <c r="B68" t="s">
-        <v>133</v>
+        <v>125</v>
       </c>
       <c r="C68" s="4">
         <v>357751000</v>
@@ -2512,7 +2512,7 @@
         <v>99</v>
       </c>
       <c r="B69" t="s">
-        <v>134</v>
+        <v>126</v>
       </c>
       <c r="C69" s="4">
         <v>16000000</v>
@@ -2523,7 +2523,7 @@
         <v>99</v>
       </c>
       <c r="B70" t="s">
-        <v>135</v>
+        <v>127</v>
       </c>
       <c r="C70" s="4">
         <v>1745838302</v>
@@ -2534,7 +2534,7 @@
         <v>99</v>
       </c>
       <c r="B71" t="s">
-        <v>136</v>
+        <v>128</v>
       </c>
       <c r="C71" s="4">
         <v>514817652</v>
@@ -2545,7 +2545,7 @@
         <v>99</v>
       </c>
       <c r="B72" t="s">
-        <v>137</v>
+        <v>129</v>
       </c>
       <c r="C72" s="4">
         <v>250000000</v>
@@ -2556,7 +2556,7 @@
         <v>99</v>
       </c>
       <c r="B73" t="s">
-        <v>138</v>
+        <v>130</v>
       </c>
       <c r="C73" s="4">
         <v>165540000</v>
@@ -2567,7 +2567,7 @@
         <v>99</v>
       </c>
       <c r="B74" t="s">
-        <v>139</v>
+        <v>131</v>
       </c>
       <c r="C74" s="4">
         <v>50000001</v>
@@ -2578,7 +2578,7 @@
         <v>99</v>
       </c>
       <c r="B75" t="s">
-        <v>140</v>
+        <v>132</v>
       </c>
       <c r="C75" s="4">
         <v>35000001</v>
@@ -2589,7 +2589,7 @@
         <v>99</v>
       </c>
       <c r="B76" t="s">
-        <v>141</v>
+        <v>133</v>
       </c>
       <c r="C76" s="4">
         <v>14277650</v>
@@ -2600,7 +2600,7 @@
         <v>99</v>
       </c>
       <c r="B77" t="s">
-        <v>142</v>
+        <v>134</v>
       </c>
       <c r="C77" s="4">
         <v>29784479</v>
@@ -2611,7 +2611,7 @@
         <v>99</v>
       </c>
       <c r="B78" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="C78" s="4">
         <v>582511100</v>
@@ -2622,7 +2622,7 @@
         <v>99</v>
       </c>
       <c r="B79" t="s">
-        <v>144</v>
+        <v>136</v>
       </c>
       <c r="C79" s="4">
         <v>119773700</v>
@@ -2633,7 +2633,7 @@
         <v>99</v>
       </c>
       <c r="B80" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="C80" s="4">
         <v>787400</v>
@@ -2644,7 +2644,7 @@
         <v>99</v>
       </c>
       <c r="B81" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C81" s="4">
         <v>341633834</v>
@@ -2655,7 +2655,7 @@
         <v>99</v>
       </c>
       <c r="B82" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="C82" s="4">
         <v>24613830</v>
@@ -2666,7 +2666,7 @@
         <v>99</v>
       </c>
       <c r="B83" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="C83" s="4">
         <v>82277166</v>
@@ -2677,7 +2677,7 @@
         <v>99</v>
       </c>
       <c r="B84" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="C84" s="4">
         <v>13425170</v>
@@ -2688,7 +2688,7 @@
         <v>99</v>
       </c>
       <c r="B85" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="C85" s="4">
         <v>118535916</v>
@@ -2699,7 +2699,7 @@
         <v>99</v>
       </c>
       <c r="B86" t="s">
-        <v>151</v>
+        <v>143</v>
       </c>
       <c r="C86" s="4">
         <v>1800000</v>
@@ -2710,7 +2710,7 @@
         <v>99</v>
       </c>
       <c r="B87" t="s">
-        <v>152</v>
+        <v>144</v>
       </c>
       <c r="C87" s="4">
         <v>38000000</v>
@@ -2721,7 +2721,7 @@
         <v>99</v>
       </c>
       <c r="B88" t="s">
-        <v>153</v>
+        <v>145</v>
       </c>
       <c r="C88" s="4">
         <v>25000000</v>
@@ -2732,7 +2732,7 @@
         <v>99</v>
       </c>
       <c r="B89" t="s">
-        <v>154</v>
+        <v>146</v>
       </c>
       <c r="C89" s="4">
         <v>12700000</v>
@@ -2743,7 +2743,7 @@
         <v>99</v>
       </c>
       <c r="B90" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C90" s="4">
         <v>200000</v>
@@ -2754,7 +2754,7 @@
         <v>99</v>
       </c>
       <c r="B91" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C91" s="4">
         <v>17490343</v>
@@ -2765,7 +2765,7 @@
         <v>99</v>
       </c>
       <c r="B92" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C92" s="4">
         <v>5500000</v>
@@ -2776,7 +2776,7 @@
         <v>99</v>
       </c>
       <c r="B93" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C93" s="4">
         <v>2500000</v>
@@ -2787,7 +2787,7 @@
         <v>99</v>
       </c>
       <c r="B94" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
       <c r="C94" s="4">
         <v>1077000</v>
@@ -2798,7 +2798,7 @@
         <v>99</v>
       </c>
       <c r="B95" t="s">
-        <v>160</v>
+        <v>152</v>
       </c>
       <c r="C95" s="4">
         <v>13268573</v>
@@ -2809,7 +2809,7 @@
         <v>99</v>
       </c>
       <c r="B96" t="s">
-        <v>161</v>
+        <v>153</v>
       </c>
       <c r="C96" s="4">
         <v>1000000</v>
@@ -2820,7 +2820,7 @@
         <v>99</v>
       </c>
       <c r="B97" t="s">
-        <v>162</v>
+        <v>154</v>
       </c>
       <c r="C97" s="4">
         <v>117920000</v>
@@ -2831,7 +2831,7 @@
         <v>99</v>
       </c>
       <c r="B98" t="s">
-        <v>163</v>
+        <v>155</v>
       </c>
       <c r="C98" s="4">
         <v>1170756762</v>
@@ -2842,7 +2842,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>164</v>
+        <v>156</v>
       </c>
       <c r="C99" s="4">
         <v>93042701</v>
@@ -2853,7 +2853,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>165</v>
+        <v>157</v>
       </c>
       <c r="C100" s="4">
         <v>15000000</v>
@@ -2864,7 +2864,7 @@
         <v>99</v>
       </c>
       <c r="B101" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="C101" s="4">
         <v>19542701</v>
@@ -2875,7 +2875,7 @@
         <v>99</v>
       </c>
       <c r="B102" t="s">
-        <v>167</v>
+        <v>159</v>
       </c>
       <c r="C102" s="4">
         <v>58500000</v>
@@ -2886,7 +2886,7 @@
         <v>99</v>
       </c>
       <c r="B103" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="C103" s="4">
         <v>435269090</v>
@@ -2897,7 +2897,7 @@
         <v>99</v>
       </c>
       <c r="B104" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C104" s="4">
         <v>82000000</v>
@@ -2908,7 +2908,7 @@
         <v>99</v>
       </c>
       <c r="B105" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C105" s="4">
         <v>233000000</v>
@@ -2919,7 +2919,7 @@
         <v>99</v>
       </c>
       <c r="B106" t="s">
-        <v>171</v>
+        <v>163</v>
       </c>
       <c r="C106" s="4">
         <v>259628210</v>
@@ -2930,7 +2930,7 @@
         <v>99</v>
       </c>
       <c r="B107" t="s">
-        <v>172</v>
+        <v>164</v>
       </c>
       <c r="C107" s="4">
         <v>101003101</v>
@@ -2941,7 +2941,7 @@
         <v>99</v>
       </c>
       <c r="B108" t="s">
-        <v>173</v>
+        <v>165</v>
       </c>
       <c r="C108" s="4">
         <v>8084596</v>
@@ -2952,7 +2952,7 @@
         <v>99</v>
       </c>
       <c r="B109" t="s">
-        <v>174</v>
+        <v>166</v>
       </c>
       <c r="C109" s="4">
         <v>27546300</v>
@@ -2963,7 +2963,7 @@
         <v>99</v>
       </c>
       <c r="B110" t="s">
-        <v>175</v>
+        <v>167</v>
       </c>
       <c r="C110" s="4">
         <v>73166702</v>
@@ -2974,7 +2974,7 @@
         <v>99</v>
       </c>
       <c r="B111" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C111" s="4">
         <v>22117660</v>
@@ -2985,7 +2985,7 @@
         <v>99</v>
       </c>
       <c r="B112" t="s">
-        <v>177</v>
+        <v>169</v>
       </c>
       <c r="C112" s="4">
         <v>27709851</v>
@@ -2996,7 +2996,7 @@
         <v>99</v>
       </c>
       <c r="B113" t="s">
-        <v>178</v>
+        <v>170</v>
       </c>
       <c r="C113" s="4">
         <v>67816761</v>
@@ -3007,7 +3007,7 @@
         <v>99</v>
       </c>
       <c r="B114" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C114" s="4">
         <v>14000000</v>
@@ -3018,7 +3018,7 @@
         <v>99</v>
       </c>
       <c r="B115" t="s">
-        <v>180</v>
+        <v>172</v>
       </c>
       <c r="C115" s="4">
         <v>7620000</v>
@@ -3029,7 +3029,7 @@
         <v>99</v>
       </c>
       <c r="B116" t="s">
-        <v>181</v>
+        <v>173</v>
       </c>
       <c r="C116" s="4">
         <v>15963900</v>
@@ -3040,7 +3040,7 @@
         <v>99</v>
       </c>
       <c r="B117" t="s">
-        <v>182</v>
+        <v>174</v>
       </c>
       <c r="C117" s="4">
         <v>19831561</v>
@@ -3051,7 +3051,7 @@
         <v>99</v>
       </c>
       <c r="B118" t="s">
-        <v>183</v>
+        <v>175</v>
       </c>
       <c r="C118" s="4">
         <v>10401300</v>
@@ -3062,7 +3062,7 @@
         <v>99</v>
       </c>
       <c r="B119" t="s">
-        <v>184</v>
+        <v>176</v>
       </c>
       <c r="C119" s="4">
         <v>2974235985</v>
@@ -3073,7 +3073,7 @@
         <v>99</v>
       </c>
       <c r="B120" t="s">
-        <v>185</v>
+        <v>177</v>
       </c>
       <c r="C120" s="4">
         <v>6193993</v>
@@ -3084,7 +3084,7 @@
         <v>99</v>
       </c>
       <c r="B121" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="C121" s="4">
         <v>906004642</v>
@@ -3095,7 +3095,7 @@
         <v>99</v>
       </c>
       <c r="B122" t="s">
-        <v>187</v>
+        <v>179</v>
       </c>
       <c r="C122" s="4">
         <v>316927183</v>
@@ -3106,7 +3106,7 @@
         <v>99</v>
       </c>
       <c r="B123" t="s">
-        <v>188</v>
+        <v>180</v>
       </c>
       <c r="C123" s="4">
         <v>23177779</v>
@@ -3117,7 +3117,7 @@
         <v>99</v>
       </c>
       <c r="B124" t="s">
-        <v>189</v>
+        <v>181</v>
       </c>
       <c r="C124" s="4">
         <v>37205000</v>
@@ -3128,7 +3128,7 @@
         <v>99</v>
       </c>
       <c r="B125" t="s">
-        <v>190</v>
+        <v>182</v>
       </c>
       <c r="C125" s="4">
         <v>80000000</v>
@@ -3139,7 +3139,7 @@
         <v>99</v>
       </c>
       <c r="B126" t="s">
-        <v>191</v>
+        <v>183</v>
       </c>
       <c r="C126" s="4">
         <v>10000000</v>
@@ -3150,7 +3150,7 @@
         <v>99</v>
       </c>
       <c r="B127" t="s">
-        <v>192</v>
+        <v>184</v>
       </c>
       <c r="C127" s="4">
         <v>43428353</v>
@@ -3161,7 +3161,7 @@
         <v>99</v>
       </c>
       <c r="B128" t="s">
-        <v>193</v>
+        <v>185</v>
       </c>
       <c r="C128" s="4">
         <v>53724050</v>
@@ -3172,7 +3172,7 @@
         <v>99</v>
       </c>
       <c r="B129" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="C129" s="4">
         <v>300000000</v>
@@ -3183,7 +3183,7 @@
         <v>99</v>
       </c>
       <c r="B130" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="C130" s="4">
         <v>41542277</v>
@@ -3194,7 +3194,7 @@
         <v>99</v>
       </c>
       <c r="B131" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="C131" s="4">
         <v>215151350</v>
@@ -3205,7 +3205,7 @@
         <v>99</v>
       </c>
       <c r="B132" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="C132" s="4">
         <v>1846886000</v>
@@ -3216,7 +3216,7 @@
         <v>99</v>
       </c>
       <c r="B133" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
       <c r="C133" s="4">
         <v>648747000</v>
@@ -3227,7 +3227,7 @@
         <v>99</v>
       </c>
       <c r="B134" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
       <c r="C134" s="4">
         <v>19684000</v>
@@ -3238,7 +3238,7 @@
         <v>99</v>
       </c>
       <c r="B135" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
       <c r="C135" s="4">
         <v>200000000</v>
@@ -3249,7 +3249,7 @@
         <v>99</v>
       </c>
       <c r="B136" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C136" s="4">
         <v>300000000</v>
@@ -3260,7 +3260,7 @@
         <v>99</v>
       </c>
       <c r="B137" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
       <c r="C137" s="4">
         <v>160000000</v>
@@ -3271,7 +3271,7 @@
         <v>99</v>
       </c>
       <c r="B138" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
       <c r="C138" s="4">
         <v>15000000</v>
@@ -3282,7 +3282,7 @@
         <v>99</v>
       </c>
       <c r="B139" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
       <c r="C139" s="4">
         <v>485000000</v>
@@ -3293,7 +3293,7 @@
         <v>99</v>
       </c>
       <c r="B140" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
       <c r="C140" s="4">
         <v>18455000</v>
@@ -3304,7 +3304,7 @@
         <v>99</v>
       </c>
       <c r="B141" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
       <c r="C141" s="4">
         <v>116229592</v>

</xml_diff>